<commit_message>
collected team data individually and reordered
</commit_message>
<xml_diff>
--- a/collected data/ipl_2025_all_teams_players_info.xlsx
+++ b/collected data/ipl_2025_all_teams_players_info.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29101"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29106"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\ipl-2025-analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\ipl-2025-analysis\collected data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{806B21EE-6E30-4274-AFF3-3D24DCDCE6F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DC8CABF-8A88-44CB-B2C9-45D9E334BC5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="952" uniqueCount="725">
   <si>
     <t>Team</t>
   </si>
@@ -523,45 +523,30 @@
     <t>Anuj Rawat</t>
   </si>
   <si>
-    <t>['FULL NAME\n\nAnuj Rawat', 'BORN\n\nOctober 17, 1999, Ram Nagar, Uttarakhand', 'AGE\n\n25y 262d', 'BATTING STYLE\n\nLeft hand Bat', 'PLAYING ROLE\n\nWicketkeeper Batter']</t>
-  </si>
-  <si>
     <t>https://www.espncricinfo.com/cricketers/anuj-rawat-1123073</t>
   </si>
   <si>
     <t>Mahipal Lomror</t>
   </si>
   <si>
-    <t>['FULL NAME\n\nMahipal Krishan Lomror', 'BORN\n\nNovember 16, 1999, Nagaur, Rajasthan', 'AGE\n\n25y 232d', 'BATTING STYLE\n\nLeft hand Bat', 'BOWLING STYLE\n\nSlow Left arm Orthodox', 'PLAYING ROLE\n\nAllrounder']</t>
-  </si>
-  <si>
     <t>https://www.espncricinfo.com/cricketers/mahipal-lomror-853265</t>
   </si>
   <si>
     <t>Sai Sudharsan</t>
   </si>
   <si>
-    <t>['FULL NAME\n\nBhardwaj Sai Sudharsan', 'BORN\n\nOctober 15, 2001, Chennai', 'AGE\n\n23y 264d', 'BATTING STYLE\n\nLeft hand Bat', 'BOWLING STYLE\n\nLegbreak', 'PLAYING ROLE\n\nTop order Batter']</t>
-  </si>
-  <si>
     <t>https://www.espncricinfo.com/cricketers/sai-sudharsan-1151288</t>
   </si>
   <si>
     <t>Dasun Shanaka</t>
   </si>
   <si>
-    <t>['FULL NAME\n\nMadagamagamage Dasun Shanaka', 'BORN\n\nSeptember 09, 1991, Negombo', 'AGE\n\n33y 300d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nRight arm Medium', 'PLAYING ROLE\n\nAllrounder', 'HEIGHT\n\n6ft', 'EDUCATION\n\nSt. Peters College - Negombo, Maristella College']</t>
-  </si>
-  <si>
     <t>https://www.espncricinfo.com/cricketers/dasun-shanaka-437316</t>
   </si>
   <si>
     <t>Washington Sundar</t>
   </si>
   <si>
-    <t>['FULL NAME\n\nWashington Sundar', 'BORN\n\nOctober 05, 1999, Chennai, Tamil Nadu', 'AGE\n\n25y 274d', 'BATTING STYLE\n\nLeft hand Bat', 'BOWLING STYLE\n\nRight arm Offbreak', 'PLAYING ROLE\n\nBowling Allrounder', 'RELATIONS\n\nM Shailaja\n\n(sister)']</t>
-  </si>
-  <si>
     <t>https://www.espncricinfo.com/cricketers/washington-sundar-719715</t>
   </si>
   <si>
@@ -619,45 +604,30 @@
     <t>Akash Singh</t>
   </si>
   <si>
-    <t>['FULL NAME\n\nAkash Maharaj Singh', 'BORN\n\nApril 26, 2002, Bharatpur, Rajasthan', 'AGE\n\n23y 71d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nLeft arm Medium fast', 'PLAYING ROLE\n\nBowler']</t>
-  </si>
-  <si>
     <t>https://www.espncricinfo.com/cricketers/akash-singh-1175458</t>
   </si>
   <si>
     <t>Yuvraj Chaudhary</t>
   </si>
   <si>
-    <t>['FULL NAME\n\nYuvraj Chaudhary', 'BORN\n\nOctober 06, 2001, Haridwar', 'AGE\n\n23y 273d', 'BATTING STYLE\n\nLeft hand Bat', 'BOWLING STYLE\n\nSlow Left arm Orthodox', 'PLAYING ROLE\n\nBatting Allrounder']</t>
-  </si>
-  <si>
     <t>https://www.espncricinfo.com/cricketers/yuvraj-chaudhary-1175463</t>
   </si>
   <si>
     <t>Arshin Kulkarni</t>
   </si>
   <si>
-    <t>['FULL NAME\n\nArshin Atul Kulkarni', 'BORN\n\nFebruary 15, 2005, Solapur, Maharashtra', 'AGE\n\n20y 141d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nRight arm Medium', 'PLAYING ROLE\n\nAllrounder']</t>
-  </si>
-  <si>
     <t>https://www.espncricinfo.com/cricketers/arshin-kulkarni-1403153</t>
   </si>
   <si>
     <t>Prince Yadav</t>
   </si>
   <si>
-    <t>['FULL NAME\n\nPrince Yadav', 'BORN\n\nDecember 12, 2001', 'AGE\n\n23y 206d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nRight arm Fast', 'PLAYING ROLE\n\nBowler']</t>
-  </si>
-  <si>
     <t>https://www.espncricinfo.com/cricketers/prince-yadav-1350768</t>
   </si>
   <si>
     <t>Ravi Bishnoi</t>
   </si>
   <si>
-    <t>['FULL NAME\n\nRavi Bishnoi', 'BORN\n\nSeptember 05, 2000, Jodhpur, Rajasthan', 'AGE\n\n24y 304d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nLegbreak Googly', 'PLAYING ROLE\n\nBowler']</t>
-  </si>
-  <si>
     <t>https://www.espncricinfo.com/cricketers/ravi-bishnoi-1175441</t>
   </si>
   <si>
@@ -667,45 +637,30 @@
     <t>Ashwani Kumar</t>
   </si>
   <si>
-    <t>['FULL NAME\n\nAshwani Kumar', 'BORN\n\nAugust 29, 2001, Jhanjeri,, Mohali', 'AGE\n\n23y 311d', 'BATTING STYLE\n\nLeft hand Bat', 'BOWLING STYLE\n\nLeft arm Medium', 'PLAYING ROLE\n\nBowler']</t>
-  </si>
-  <si>
     <t>https://www.espncricinfo.com/cricketers/ashwani-kumar-1209126</t>
   </si>
   <si>
     <t>Raj Bawa</t>
   </si>
   <si>
-    <t>['FULL NAME\n\nRaj\xa0Angad\xa0Bawa', 'BORN\n\nNovember 12, 2002, Nahan, Himachal Pradesh', 'AGE\n\n22y 236d', 'BATTING STYLE\n\nLeft hand Bat', 'BOWLING STYLE\n\nRight arm Medium fast', 'PLAYING ROLE\n\nAllrounder']</t>
-  </si>
-  <si>
     <t>https://www.espncricinfo.com/cricketers/raj-bawa-1292502</t>
   </si>
   <si>
     <t>Corbin Bosch</t>
   </si>
   <si>
-    <t>['FULL NAME\n\nCorbin Bosch', 'BORN\n\nSeptember 10, 1994, Durban', 'AGE\n\n30y 299d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nRight arm Fast medium', 'PLAYING ROLE\n\nAllrounder', 'RELATIONS\n\nT Bosch\n\n(father),\n\nE Bosch\n\n(brother)']</t>
-  </si>
-  <si>
     <t>https://www.espncricinfo.com/cricketers/corbin-bosch-594322</t>
   </si>
   <si>
     <t>Satyanarayana Raju</t>
   </si>
   <si>
-    <t>['FULL NAME\n\nPenumatsa Venkata Satyanarayana Raju', 'BORN\n\nJuly 10, 1999', 'AGE\n\n25y 361d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nRight arm Medium fast', 'PLAYING ROLE\n\nBowler', 'RELATIONS\n\nPP Raju\n\n(brother)']</t>
-  </si>
-  <si>
     <t>https://www.espncricinfo.com/cricketers/satyanarayana-raju-1392201</t>
   </si>
   <si>
     <t>Karn Sharma</t>
   </si>
   <si>
-    <t>['FULL NAME\n\nKarn Vinod Sharma', 'BORN\n\nOctober 23, 1987, Meerut, Uttar Pradesh', 'AGE\n\n37y 256d', 'BATTING STYLE\n\nLeft hand Bat', 'BOWLING STYLE\n\nLegbreak Googly', 'PLAYING ROLE\n\nBowler']</t>
-  </si>
-  <si>
     <t>https://www.espncricinfo.com/cricketers/karn-sharma-30288</t>
   </si>
   <si>
@@ -1162,45 +1117,30 @@
     <t>Manoj Bhandage</t>
   </si>
   <si>
-    <t>['FULL NAME\n\nManoj Shivaramsa Bhandage', 'BORN\n\nOctober 05, 1998, Raichur, Karnataka', 'AGE\n\n26y 274d', 'BATTING STYLE\n\nLeft hand Bat', 'BOWLING STYLE\n\nRight arm Medium fast', 'PLAYING ROLE\n\nAllrounder']</t>
-  </si>
-  <si>
     <t>https://www.espncricinfo.com/cricketers/manoj-bhandage-1057399</t>
   </si>
   <si>
     <t>Rajat Patidar</t>
   </si>
   <si>
-    <t>['FULL NAME\n\nRajat Manohar Patidar', 'BORN\n\nJune 01, 1993, Indore, Madhya Pradesh', 'AGE\n\n32y 35d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nRight arm Offbreak', 'PLAYING ROLE\n\nTop order Batter']</t>
-  </si>
-  <si>
     <t>https://www.espncricinfo.com/cricketers/rajat-patidar-823703</t>
   </si>
   <si>
     <t>Rasikh Salam</t>
   </si>
   <si>
-    <t>['FULL NAME\n\nRasikh Salam Dar', 'BORN\n\nApril 05, 2000', 'AGE\n\n25y 92d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nRight arm Medium', 'PLAYING ROLE\n\nBowler']</t>
-  </si>
-  <si>
     <t>https://www.espncricinfo.com/cricketers/rasikh-salam-1161489</t>
   </si>
   <si>
     <t>Tim Seifert</t>
   </si>
   <si>
-    <t>['FULL NAME\n\nTim Louis Seifert', 'BORN\n\nDecember 14, 1994, Wanganui', 'AGE\n\n30y 204d', 'BATTING STYLE\n\nRight hand Bat', 'FIELDING POSITION\n\nWicketkeeper', 'PLAYING ROLE\n\nWicketkeeper Batter']</t>
-  </si>
-  <si>
     <t>https://www.espncricinfo.com/cricketers/tim-seifert-625964</t>
   </si>
   <si>
     <t>Swapnil Singh</t>
   </si>
   <si>
-    <t>['FULL NAME\n\nSwapnil Singh', 'BORN\n\nJanuary 22, 1991, Rae Bareilly, Uttar Pradesh', 'AGE\n\n34y 165d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nSlow Left arm Orthodox', 'PLAYING ROLE\n\nBowler']</t>
-  </si>
-  <si>
     <t>https://www.espncricinfo.com/cricketers/swapnil-singh-232292</t>
   </si>
   <si>
@@ -1250,6 +1190,1011 @@
   </si>
   <si>
     <t>https://www.espncricinfo.com/cricketers/zeeshan-ansari-942371</t>
+  </si>
+  <si>
+    <t>Ajinkya Rahane</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nAjinkya Madhukar Rahane', 'BORN\n\nJune 06, 1988, Ashwi-KD, Maharashtra', 'AGE\n\n37y 30d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nRight arm Medium', 'PLAYING ROLE\n\nTop order Batter']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/ajinkya-rahane-277916</t>
+  </si>
+  <si>
+    <t>Quinton de Kock</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nQuinton de Kock', 'BORN\n\nDecember 17, 1992, Johannesburg, Gauteng', 'AGE\n\n32y 201d', 'BATTING STYLE\n\nLeft hand Bat', 'FIELDING POSITION\n\nWicketkeeper', 'PLAYING ROLE\n\nWicketkeeper Batter']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/quinton-de-kock-379143</t>
+  </si>
+  <si>
+    <t>Manish Pandey</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nManish Krishnanand Pandey', 'BORN\n\nSeptember 10, 1989, Nainital, Uttaranchal', 'AGE\n\n35y 299d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nRight arm Medium', 'PLAYING ROLE\n\nTop order Batter']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/manish-pandey-290630</t>
+  </si>
+  <si>
+    <t>Rahmanullah Gurbaz</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nRahmanullah Gurbaz', 'BORN\n\nNovember 28, 2001', 'AGE\n\n23y 220d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nRight arm Medium', 'FIELDING POSITION\n\nWicketkeeper', 'PLAYING ROLE\n\nWicketkeeper Batter', 'RELATIONS\n\nMasood Gurbaz\n\n(brother)']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/rahmanullah-gurbaz-974087</t>
+  </si>
+  <si>
+    <t>Ramandeep Singh</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nRamandeep Singh', 'BORN\n\nApril 13, 1997, Chandigarh', 'AGE\n\n28y 84d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nRight arm Medium', 'PLAYING ROLE\n\nMiddle order Batter']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/ramandeep-singh-1079470</t>
+  </si>
+  <si>
+    <t>Rinku Singh</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nRinku Khanchand Singh', 'BORN\n\nOctober 12, 1997, Aligarh, Uttar Pradesh', 'AGE\n\n27y 267d', 'BATTING STYLE\n\nLeft hand Bat', 'BOWLING STYLE\n\nRight arm Offbreak', 'PLAYING ROLE\n\nMiddle order Batter']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/rinku-singh-723105</t>
+  </si>
+  <si>
+    <t>Rovman Powell</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nRovman Powell', 'BORN\n\nJuly 23, 1993, Jamaica', 'AGE\n\n31y 348d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nRight arm Medium fast', 'PLAYING ROLE\n\nMiddle order Batter']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/rovman-powell-820351</t>
+  </si>
+  <si>
+    <t>Sunil Narine</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nSunil Philip Narine', 'BORN\n\nMay 26, 1988, Arima, Trinidad &amp; Tobago', 'AGE\n\n37y 41d', 'BATTING STYLE\n\nLeft hand Bat', 'BOWLING STYLE\n\nRight arm Offbreak', 'PLAYING ROLE\n\nBowling Allrounder']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/sunil-narine-230558</t>
+  </si>
+  <si>
+    <t>Andre Russell</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nAndre Dwayne Russell', 'BORN\n\nApril 29, 1988, Jamaica', 'AGE\n\n37y 68d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nRight arm Fast', 'PLAYING ROLE\n\nAllrounder']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/andre-russell-276298</t>
+  </si>
+  <si>
+    <t>Moeen Ali</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nMoeen Munir Ali', 'BORN\n\nJune 18, 1987, Birmingham', 'AGE\n\n38y 18d', 'NICKNAMES\n\nMoe', 'BATTING STYLE\n\nLeft hand Bat', 'BOWLING STYLE\n\nRight arm Offbreak', 'PLAYING ROLE\n\nBatting Allrounder', 'HEIGHT\n\n6ft', 'EDUCATION\n\nMoseley School', 'RELATIONS\n\nOM Ali\n\n(brother),\n\nKabir Ali\n\n(cousin),\n\nKadeer Ali\n\n(brother),\n\nA Ali\n\n(cousin)']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/moeen-ali-8917</t>
+  </si>
+  <si>
+    <t>Vaibhav Arora</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nVaibhav Gopal Arora', 'BORN\n\nDecember 14, 1997', 'AGE\n\n27y 204d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nRight arm Fast medium', 'PLAYING ROLE\n\nBowler']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/vaibhav-arora-1209292</t>
+  </si>
+  <si>
+    <t>Harshit Rana</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nHarshit Pradeep Rana', 'BORN\n\nDecember 22, 2001, New Delhi', 'AGE\n\n23y 196d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nRight arm Fast', 'PLAYING ROLE\n\nBowler']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/harshit-rana-1312645</t>
+  </si>
+  <si>
+    <t>Mayank Markande</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nMayank Markande', 'BORN\n\nNovember 11, 1997, Bathinda, Punjab', 'AGE\n\n27y 237d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nLegbreak', 'PLAYING ROLE\n\nBowler']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/mayank-markande-1081442</t>
+  </si>
+  <si>
+    <t>Anrich Nortje</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nAnrich Arno Nortje', 'BORN\n\nNovember 16, 1993', 'AGE\n\n31y 232d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nRight arm Fast', 'PLAYING ROLE\n\nBowler']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/anrich-nortje-481979</t>
+  </si>
+  <si>
+    <t>Chetan Sakariya</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nChetan Sakariya', 'BORN\n\nFebruary 28, 1998, Bhavnagar', 'AGE\n\n27y 128d', 'BATTING STYLE\n\nLeft hand Bat', 'BOWLING STYLE\n\nLeft arm Medium fast', 'PLAYING ROLE\n\nBowler']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/chetan-sakariya-1131754</t>
+  </si>
+  <si>
+    <t>Varun Chakravarthy</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nVarun Chakravarthy Vinod', 'BORN\n\nAugust 29, 1991, Bidar, Karnataka', 'AGE\n\n33y 311d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nLegbreak Googly', 'PLAYING ROLE\n\nBowler']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/varun-chakravarthy-1108375</t>
+  </si>
+  <si>
+    <t>Umran Malik</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nUmran Malik', 'BORN\n\nNovember 22, 1999, Gujjar Nagar, Jammu &amp; Kashmir', 'AGE\n\n25y 226d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nRight arm Fast', 'PLAYING ROLE\n\nBowler']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/umran-malik-1246528</t>
+  </si>
+  <si>
+    <t>Shivam Shukla</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nShivam Shukla', 'BORN\n\nDecember 11, 1995, Panna', 'AGE\n\n29y 207d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nLegbreak']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/shivam-shukla-1460342</t>
+  </si>
+  <si>
+    <t>Shubman Gill</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nShubman Gill', 'BORN\n\nSeptember 08, 1999, Fazilka, Punjab', 'AGE\n\n25y 303d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nRight arm Offbreak', 'PLAYING ROLE\n\nMiddle order Batter']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/shubman-gill-1070173</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nAnuj Rawat', 'BORN\n\nOctober 17, 1999, Ram Nagar, Uttarakhand', 'AGE\n\n25y 264d', 'BATTING STYLE\n\nLeft hand Bat', 'PLAYING ROLE\n\nWicketkeeper Batter']</t>
+  </si>
+  <si>
+    <t>Kumar Kushagra</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nKumar Kushagra', 'BORN\n\nOctober 23, 2004, Bokaro, Jharkhand', 'AGE\n\n20y 258d', 'BATTING STYLE\n\nRight hand Bat', 'FIELDING POSITION\n\nWicketkeeper', 'PLAYING ROLE\n\nWicketkeeper Batter']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/kumar-kushagra-1207295</t>
+  </si>
+  <si>
+    <t>Kusal Mendis</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nBalapuwaduge Kusal Gimhan Mendis', 'BORN\n\nFebruary 02, 1995, Moratuwa', 'AGE\n\n30y 156d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nLegbreak', 'FIELDING POSITION\n\nWicketkeeper', 'PLAYING ROLE\n\nWicketkeeper Batter', 'EDUCATION\n\nPrince of Wales College, Moratuwa', 'RELATIONS\n\nBOL Mendis\n\n(brother)']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/kusal-mendis-629074</t>
+  </si>
+  <si>
+    <t>Sherfane Rutherford</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nSherfane Eviston Rutherford', 'BORN\n\nAugust 15, 1998', 'AGE\n\n26y 327d', 'BATTING STYLE\n\nLeft hand Bat', 'BOWLING STYLE\n\nRight arm Fast medium', 'PLAYING ROLE\n\nMiddle order Batter']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/sherfane-rutherford-914541</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nBhardwaj Sai Sudharsan', 'BORN\n\nOctober 15, 2001, Chennai', 'AGE\n\n23y 266d', 'BATTING STYLE\n\nLeft hand Bat', 'BOWLING STYLE\n\nLegbreak', 'PLAYING ROLE\n\nTop order Batter']</t>
+  </si>
+  <si>
+    <t>M Shahrukh Khan</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nMasood Shahrukh Khan', 'BORN\n\nMay 27, 1995, Chennai, Tamil Nadu', 'AGE\n\n30y 42d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nRight arm Offbreak', 'PLAYING ROLE\n\nBatter']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/m-shahrukh-khan-719719</t>
+  </si>
+  <si>
+    <t>Jos Buttler</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nJoseph Charles Buttler', 'BORN\n\nSeptember 08, 1990, Taunton, Somerset', 'AGE\n\n34y 303d', 'BATTING STYLE\n\nRight hand Bat', 'FIELDING POSITION\n\nWicketkeeper', 'PLAYING ROLE\n\nWicketkeeper Batter', "EDUCATION\n\nKing's College, Taunton"]</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/jos-buttler-308967</t>
+  </si>
+  <si>
+    <t>Rashid Khan</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nRashid Khan Arman', 'BORN\n\nSeptember 20, 1998, Nangarhar', 'AGE\n\n26y 291d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nLegbreak Googly', 'PLAYING ROLE\n\nBowling Allrounder', 'RELATIONS\n\nUsman Khan Shinwari\n\n(nephew)']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/rashid-khan-793463</t>
+  </si>
+  <si>
+    <t>Karim Janat</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nKarim Janat', 'BORN\n\nAugust 11, 1998, Kabul', 'AGE\n\n26y 331d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nRight arm Medium', 'PLAYING ROLE\n\nBowling Allrounder', 'RELATIONS\n\nAsghar Afghan\n\n(brother)']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/karim-janat-793467</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nMahipal Krishan Lomror', 'BORN\n\nNovember 16, 1999, Nagaur, Rajasthan', 'AGE\n\n25y 234d', 'BATTING STYLE\n\nLeft hand Bat', 'BOWLING STYLE\n\nSlow Left arm Orthodox', 'PLAYING ROLE\n\nAllrounder']</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nMadagamagamage Dasun Shanaka', 'BORN\n\nSeptember 09, 1991, Negombo', 'AGE\n\n33y 302d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nRight arm Medium', 'PLAYING ROLE\n\nAllrounder', 'HEIGHT\n\n6ft', 'EDUCATION\n\nSt. Peters College - Negombo, Maristella College']</t>
+  </si>
+  <si>
+    <t>Nishant Sindhu</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nNishant Sindhu', 'BORN\n\nApril 09, 2004, Rohtak, Haryana', 'AGE\n\n21y 90d', 'BATTING STYLE\n\nLeft hand Bat', 'BOWLING STYLE\n\nSlow Left arm Orthodox', 'PLAYING ROLE\n\nAllrounder']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/nishant-sindhu-1292506</t>
+  </si>
+  <si>
+    <t>Manav Suthar</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nManav Jagdusakumar Suthar', 'BORN\n\nAugust 03, 2002, Sri Ganganagar, Rajasthan', 'AGE\n\n22y 339d', 'BATTING STYLE\n\nLeft hand Bat', 'BOWLING STYLE\n\nSlow Left arm Orthodox', 'PLAYING ROLE\n\nBowling Allrounder']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/manav-suthar-1175426</t>
+  </si>
+  <si>
+    <t>Rahul Tewatia</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nRahul Tewatia', 'BORN\n\nMay 20, 1993, Sihi, Haryana', 'AGE\n\n32y 49d', 'BATTING STYLE\n\nLeft hand Bat', 'BOWLING STYLE\n\nLegbreak', 'PLAYING ROLE\n\nBowling Allrounder']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/rahul-tewatia-423838</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nWashington Sundar', 'BORN\n\nOctober 05, 1999, Chennai, Tamil Nadu', 'AGE\n\n25y 276d', 'BATTING STYLE\n\nLeft hand Bat', 'BOWLING STYLE\n\nRight arm Offbreak', 'PLAYING ROLE\n\nBowling Allrounder', 'RELATIONS\n\nM Shailaja\n\n(sister)']</t>
+  </si>
+  <si>
+    <t>Glenn Phillips</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nGlenn Dominic Phillips', 'BORN\n\nDecember 06, 1996, East London, Eastern Cape, South Africa', 'AGE\n\n28y 214d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nRight arm Offbreak', 'FIELDING POSITION\n\nWicketkeeper', 'PLAYING ROLE\n\nAllrounder', 'RELATIONS\n\nDJ Grobbelaar\n\n(brother-in-law),\n\nDN Phillips\n\n(brother)']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/glenn-phillips-823509</t>
+  </si>
+  <si>
+    <t>Arshad Khan</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nMohd Arshad Khan', 'BORN\n\nDecember 20, 1997, Gopalganj (Seoni)', 'AGE\n\n27y 200d', 'BATTING STYLE\n\nLeft hand Bat', 'BOWLING STYLE\n\nLeft arm Fast medium', 'PLAYING ROLE\n\nBowler']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/arshad-khan-1244751</t>
+  </si>
+  <si>
+    <t>Gerald Coetzee</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nGerald Coetzee', 'BORN\n\nOctober 02, 2000', 'AGE\n\n24y 279d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nRight arm Fast', 'PLAYING ROLE\n\nBowler', 'EDUCATION\n\nSaint Andrews School']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/gerald-coetzee-596010</t>
+  </si>
+  <si>
+    <t>Gurnoor Brar</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nGurnoor Brar', 'BORN\n\nMay 25, 2000, Muktsar, Punjab', 'AGE\n\n25y 44d', 'BATTING STYLE\n\nLeft hand Bat', 'BOWLING STYLE\n\nRight arm Fast', 'PLAYING ROLE\n\nBowler']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/gurnoor-brar-1287033</t>
+  </si>
+  <si>
+    <t>Kulwant Khejroliya</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nKulwant Khejroliya', 'BORN\n\nMarch 13, 1992, Churi Ajitgarh Jhunjhunu District, Rajasthan', 'AGE\n\n33y 117d', 'BATTING STYLE\n\nLeft hand Bat', 'BOWLING STYLE\n\nLeft arm Medium fast', 'PLAYING ROLE\n\nBowler']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/kulwant-khejroliya-1083033</t>
+  </si>
+  <si>
+    <t>Mohammed Siraj</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nMohammed Siraj', 'BORN\n\nMarch 13, 1994, Hyderabad', 'AGE\n\n31y 117d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nRight arm Fast', 'PLAYING ROLE\n\nBowler']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/mohammed-siraj-940973</t>
+  </si>
+  <si>
+    <t>Prasidh Krishna</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nMuralikrishna Prasidh Krishna', 'BORN\n\nFebruary 19, 1996, Bangalore, Karnataka', 'AGE\n\n29y 139d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nRight arm Fast medium', 'PLAYING ROLE\n\nBowler']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/prasidh-krishna-917159</t>
+  </si>
+  <si>
+    <t>Kagiso Rabada</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nKagiso Rabada', 'BORN\n\nMay 25, 1995, Johannesburg', 'AGE\n\n30y 44d', 'BATTING STYLE\n\nLeft hand Bat', 'BOWLING STYLE\n\nRight arm Fast', 'PLAYING ROLE\n\nBowler']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/kagiso-rabada-550215</t>
+  </si>
+  <si>
+    <t>Sai Kishore</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nRavisrinivasan Sai Kishore', 'BORN\n\nNovember 06, 1996, Chennai, Tamil Nadu', 'AGE\n\n28y 244d', 'BATTING STYLE\n\nLeft hand Bat', 'BOWLING STYLE\n\nSlow Left arm Orthodox', 'PLAYING ROLE\n\nBowler']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/sai-kishore-1048739</t>
+  </si>
+  <si>
+    <t>Ishant Sharma</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nIshant Sharma', 'BORN\n\nSeptember 02, 1988, Delhi', 'AGE\n\n36y 309d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nRight arm Fast medium', 'PLAYING ROLE\n\nBowler']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/ishant-sharma-236779</t>
+  </si>
+  <si>
+    <t>Jayant Yadav</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nJayant Yadav', 'BORN\n\nJanuary 22, 1990, Delhi', 'AGE\n\n35y 167d', 'ALSO KNOWN AS\n\nJayant Yadav', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nRight arm Offbreak', 'PLAYING ROLE\n\nBowler']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/jayant-yadav-447587</t>
+  </si>
+  <si>
+    <t>Rishabh Pant</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nRishabh Rajendra Pant', 'BORN\n\nOctober 04, 1997, Haridwar, Uttarakhand', 'AGE\n\n27y 277d', 'BATTING STYLE\n\nLeft hand Bat', 'FIELDING POSITION\n\nWicketkeeper', 'PLAYING ROLE\n\nWicketkeeper Batter']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/rishabh-pant-931581</t>
+  </si>
+  <si>
+    <t>Abdul Samad</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nAbdul Samad Farooq', 'BORN\n\nOctober 28, 2001, Kala Kot, Jammu &amp; Kashmir', 'AGE\n\n23y 253d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nLegbreak', 'PLAYING ROLE\n\nBatter']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/abdul-samad-1175485</t>
+  </si>
+  <si>
+    <t>Ayush Badoni</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nAyush Badoni', 'BORN\n\nDecember 03, 1999, Delhi', 'AGE\n\n25y 217d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nRight arm Offbreak', 'PLAYING ROLE\n\nBatter']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/ayush-badoni-1151270</t>
+  </si>
+  <si>
+    <t>Matthew Breetzke</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nMatthew Paul Breetzke', 'BORN\n\nNovember 03, 1998', 'AGE\n\n26y 247d', 'BATTING STYLE\n\nRight hand Bat', 'FIELDING POSITION\n\nWicketkeeper', 'PLAYING ROLE\n\nBatter', 'EDUCATION\n\nGrey High School']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/matthew-breetzke-595267</t>
+  </si>
+  <si>
+    <t>Himmat Singh</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nHimmat Singh', 'BORN\n\nNovember 08, 1996, Delhi', 'AGE\n\n28y 242d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nRight arm Offbreak', 'PLAYING ROLE\n\nBatter']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/himmat-singh-805235</t>
+  </si>
+  <si>
+    <t>Aryan Juyal</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nAryan Juyal', 'BORN\n\nNovember 11, 2001, Moradabad, Uttar Pradesh', 'AGE\n\n23y 239d', 'BATTING STYLE\n\nRight hand Bat', 'FIELDING POSITION\n\nWicketkeeper', 'PLAYING ROLE\n\nWicketkeeper Batter']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/aryan-juyal-1130300</t>
+  </si>
+  <si>
+    <t>David Miller</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nDavid Andrew Miller', 'BORN\n\nJune 10, 1989, Pietermaritzburg, Natal', 'AGE\n\n36y 28d', 'BATTING STYLE\n\nLeft hand Bat', 'BOWLING STYLE\n\nRight arm Offbreak', 'PLAYING ROLE\n\nMiddle order Batter']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/david-miller-321777</t>
+  </si>
+  <si>
+    <t>Nicholas Pooran</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nNicholas Pooran', 'BORN\n\nOctober 02, 1995, Trinidad', 'AGE\n\n29y 279d', 'BATTING STYLE\n\nLeft hand Bat', 'BOWLING STYLE\n\nRight arm Offbreak', 'FIELDING POSITION\n\nWicketkeeper', 'PLAYING ROLE\n\nWicketkeeper Batter']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/nicholas-pooran-604302</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nYuvraj Chaudhary', 'BORN\n\nOctober 06, 2001, Haridwar', 'AGE\n\n23y 275d', 'BATTING STYLE\n\nLeft hand Bat', 'BOWLING STYLE\n\nSlow Left arm Orthodox', 'PLAYING ROLE\n\nBatting Allrounder']</t>
+  </si>
+  <si>
+    <t>Rajvardhan Hangargekar</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nRajvardhan S Hangargekar', 'BORN\n\nNovember 10, 2002, Tuljapur, Maharashtra', 'AGE\n\n22y 240d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nRight arm Fast medium', 'PLAYING ROLE\n\nBowling Allrounder']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/rajvardhan-hangargekar-1175429</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nArshin Atul Kulkarni', 'BORN\n\nFebruary 15, 2005, Solapur, Maharashtra', 'AGE\n\n20y 143d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nRight arm Medium', 'PLAYING ROLE\n\nAllrounder']</t>
+  </si>
+  <si>
+    <t>Aiden Markram</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nAiden Kyle Markram', 'BORN\n\nOctober 04, 1994, Centurion', 'AGE\n\n30y 277d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nRight arm Offbreak', 'PLAYING ROLE\n\nAllrounder']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/aiden-markram-600498</t>
+  </si>
+  <si>
+    <t>Mitchell Marsh</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nMitchell Ross Marsh', 'BORN\n\nOctober 20, 1991, Attadale, Perth', 'AGE\n\n33y 261d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nRight arm Medium', 'PLAYING ROLE\n\nAllrounder', 'RELATIONS\n\nGR Marsh\n\n(father),\n\nSE Marsh\n\n(brother)']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/mitchell-marsh-272450</t>
+  </si>
+  <si>
+    <t>Shahbaz Ahmed</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nShahbaz Ahmed', 'BORN\n\nDecember 11, 1994, Mewat, Haryana', 'AGE\n\n30y 209d', 'BATTING STYLE\n\nLeft hand Bat', 'BOWLING STYLE\n\nSlow Left arm Orthodox', 'PLAYING ROLE\n\nAllrounder']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/shahbaz-ahmed-1159711</t>
+  </si>
+  <si>
+    <t>Akash Deep</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nAkash Deep', 'BORN\n\nDecember 15, 1996, Dehri, (Rotas), Bihar', 'AGE\n\n28y 205d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nRight arm Fast medium', 'PLAYING ROLE\n\nBowler']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/akash-deep-1176959</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nAkash Maharaj Singh', 'BORN\n\nApril 26, 2002, Bharatpur, Rajasthan', 'AGE\n\n23y 73d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nLeft arm Medium fast', 'PLAYING ROLE\n\nBowler']</t>
+  </si>
+  <si>
+    <t>Avesh Khan</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nAvesh Khan', 'BORN\n\nDecember 13, 1996, Indore, Madhya Pradesh', 'AGE\n\n28y 207d', 'ALSO KNOWN AS\n\nAvesh Khan', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nRight arm Fast medium', 'PLAYING ROLE\n\nBowler']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/avesh-khan-694211</t>
+  </si>
+  <si>
+    <t>Will O’Rourke</t>
+  </si>
+  <si>
+    <t>["FULL NAME\n\nWilliam Peter O'Rourke", 'BORN\n\nAugust 06, 2001, Kingston upon Thames, Surrey', 'AGE\n\n23y 336d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nRight arm Fast', 'PLAYING ROLE\n\nBowler']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/will-o-rourke-1211825</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nPrince Yadav', 'BORN\n\nDecember 12, 2001', 'AGE\n\n23y 208d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nRight arm Fast', 'PLAYING ROLE\n\nBowler']</t>
+  </si>
+  <si>
+    <t>Digvesh Rathi</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nDigvesh Singh Rathi', 'BORN\n\nDecember 15, 1999, Delhi', 'AGE\n\n25y 205d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nLegbreak', 'PLAYING ROLE\n\nBowler']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/digvesh-rathi-1460529</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nRavi Bishnoi', 'BORN\n\nSeptember 05, 2000, Jodhpur, Rajasthan', 'AGE\n\n24y 306d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nLegbreak Googly', 'PLAYING ROLE\n\nBowler']</t>
+  </si>
+  <si>
+    <t>Manimaran Siddharth</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nManimaran Siddharth', 'BORN\n\nJuly 03, 1998', 'AGE\n\n27y 5d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nSlow Left arm Orthodox', 'PLAYING ROLE\n\nBowler']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/manimaran-siddharth-1151286</t>
+  </si>
+  <si>
+    <t>Shardul Thakur</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nShardul Narendra Thakur', 'BORN\n\nOctober 16, 1991, Palghar, Maharashtra', 'AGE\n\n33y 265d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nRight arm Medium', 'PLAYING ROLE\n\nBowler']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/shardul-thakur-475281</t>
+  </si>
+  <si>
+    <t>Shamar Joseph</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nShamar Joseph', 'BORN\n\nAugust 31, 1999', 'AGE\n\n25y 311d', 'BATTING STYLE\n\nLeft hand Bat', 'BOWLING STYLE\n\nRight arm Fast', 'PLAYING ROLE\n\nBowler']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/shamar-joseph-1356971</t>
+  </si>
+  <si>
+    <t>Mohsin Khan</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nMohsin Khan', 'BORN\n\nJuly 15, 1998, Sambhal, Uttar Pradesh', 'AGE\n\n26y 358d', 'BATTING STYLE\n\nLeft hand Bat', 'BOWLING STYLE\n\nLeft arm Medium fast', 'PLAYING ROLE\n\nBowler']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/mohsin-khan-1132005</t>
+  </si>
+  <si>
+    <t>Mayank Yadav</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nMayank Prabhu Yadav', 'BORN\n\nJune 17, 2002, New Delhi', 'AGE\n\n23y 21d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nRight arm Fast', 'PLAYING ROLE\n\nBowler']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/mayank-yadav-1292563</t>
+  </si>
+  <si>
+    <t>Jonny Bairstow</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nJonathan Marc Bairstow', 'BORN\n\nSeptember 26, 1989, Bradford, Yorkshire', 'AGE\n\n35y 285d', 'NICKNAMES\n\nBluey', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nRight arm Medium', 'FIELDING POSITION\n\nWicketkeeper', 'PLAYING ROLE\n\nWicketkeeper Batter', 'RELATIONS\n\nDL Bairstow\n\n(father),\n\nAD Bairstow\n\n(brother)']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/jonny-bairstow-297433</t>
+  </si>
+  <si>
+    <t>Bevon Jacobs</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nBevon-John Jacobs', 'BORN\n\nMay 06, 2002, Pretoria, Gauteng', 'AGE\n\n23y 63d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nRight arm Medium', 'PLAYING ROLE\n\nMiddle order Batter']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/bevon-jacobs-1410577</t>
+  </si>
+  <si>
+    <t>Robin Minz</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nRobin Minz', 'BORN\n\nSeptember 13, 2002', 'AGE\n\n22y 298d', 'BATTING STYLE\n\nLeft hand Bat', 'BOWLING STYLE\n\nSlow Left arm Orthodox', 'FIELDING POSITION\n\nWicketkeeper', 'PLAYING ROLE\n\nWicketkeeper']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/robin-minz-1350762</t>
+  </si>
+  <si>
+    <t>Naman Dhir</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nNaman Dhir', 'BORN\n\nDecember 31, 1999, Ambala, Haryana', 'AGE\n\n25y 189d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nRight arm Offbreak', 'PLAYING ROLE\n\nTop order Batter']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/naman-dhir-1287032</t>
+  </si>
+  <si>
+    <t>Rohit Sharma</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nRohit Gurunath Sharma', 'BORN\n\nApril 30, 1987, Bansod, Nagpur, Maharashtra', 'AGE\n\n38y 69d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nRight arm Offbreak', 'PLAYING ROLE\n\nTop order Batter']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/rohit-sharma-34102</t>
+  </si>
+  <si>
+    <t>Krishnan Shrijith</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nKrishnan Lakshmanan Shrijith', 'BORN\n\nAugust 12, 1996, Bangalore, Karnataka', 'AGE\n\n28y 330d', 'BATTING STYLE\n\nLeft hand Bat', 'BOWLING STYLE\n\nRight arm Offbreak', 'PLAYING ROLE\n\nWicketkeeper Batter']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/krishnan-shrijith-778241</t>
+  </si>
+  <si>
+    <t>Suryakumar Yadav</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nSuryakumar Ashok Yadav', 'BORN\n\nSeptember 14, 1990, Mumbai, Maharashtra', 'AGE\n\n34y 297d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nRight arm Medium, Right arm Offbreak', 'PLAYING ROLE\n\nBatter']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/suryakumar-yadav-446507</t>
+  </si>
+  <si>
+    <t>Ryan Rickelton</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nRyan David Rickelton', 'BORN\n\nJuly 11, 1996, Johannesburg, Transvaal, South Africa', 'AGE\n\n28y 362d', 'BATTING STYLE\n\nLeft hand Bat', 'FIELDING POSITION\n\nWicketkeeper', 'PLAYING ROLE\n\nWicketkeeper Batter', 'EDUCATION\n\nSt Stithians College']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/ryan-rickelton-605661</t>
+  </si>
+  <si>
+    <t>Hardik Pandya</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nHardik Himanshu Pandya', 'BORN\n\nOctober 11, 1993, Choryasi, Gujarat', 'AGE\n\n31y 270d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nRight arm Medium fast', 'PLAYING ROLE\n\nAllrounder', 'RELATIONS\n\nKH Pandya\n\n(brother)']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/hardik-pandya-625371</t>
+  </si>
+  <si>
+    <t>Charith Asalanka</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nKariyawasam Indipalage Charith Asalanka', 'BORN\n\nJune 29, 1997, Elpitiya', 'AGE\n\n28y 9d', 'BATTING STYLE\n\nLeft hand Bat', 'BOWLING STYLE\n\nRight arm Offbreak', 'PLAYING ROLE\n\nBatting Allrounder', 'EDUCATION\n\nRichmond College, Galle']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/charith-asalanka-784367</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nRaj\xa0Angad\xa0Bawa', 'BORN\n\nNovember 12, 2002, Nahan, Himachal Pradesh', 'AGE\n\n22y 238d', 'BATTING STYLE\n\nLeft hand Bat', 'BOWLING STYLE\n\nRight arm Medium fast', 'PLAYING ROLE\n\nAllrounder']</t>
+  </si>
+  <si>
+    <t>Mitchell Santner</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nMitchell Josef Santner', 'BORN\n\nFebruary 05, 1992, Hamilton', 'AGE\n\n33y 153d', 'BATTING STYLE\n\nLeft hand Bat', 'BOWLING STYLE\n\nSlow Left arm Orthodox', 'PLAYING ROLE\n\nBowling Allrounder', 'RELATIONS\n\nEH Santner\n\n(brother)']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/mitchell-santner-502714</t>
+  </si>
+  <si>
+    <t>Tilak Varma</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nNamboori Thakur Tilak Varma', 'BORN\n\nNovember 08, 2002, Hyderabad, Andhra Pradesh', 'AGE\n\n22y 242d', 'BATTING STYLE\n\nLeft hand Bat', 'BOWLING STYLE\n\nRight arm Offbreak', 'PLAYING ROLE\n\nBatting Allrounder']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/tilak-varma-1170265</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nCorbin Bosch', 'BORN\n\nSeptember 10, 1994, Durban', 'AGE\n\n30y 301d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nRight arm Fast medium', 'PLAYING ROLE\n\nAllrounder', 'RELATIONS\n\nT Bosch\n\n(father),\n\nE Bosch\n\n(brother)']</t>
+  </si>
+  <si>
+    <t>Will Jacks</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nWilliam George Jacks', 'BORN\n\nNovember 21, 1998, Chertsey, Surrey', 'AGE\n\n26y 229d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nRight arm Offbreak', 'PLAYING ROLE\n\nBatting Allrounder', "EDUCATION\n\nSt George's College, Weybridge"]</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/will-jacks-897549</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nAshwani Kumar', 'BORN\n\nAugust 29, 2001, Jhanjeri,, Mohali', 'AGE\n\n23y 313d', 'BATTING STYLE\n\nLeft hand Bat', 'BOWLING STYLE\n\nLeft arm Medium', 'PLAYING ROLE\n\nBowler']</t>
+  </si>
+  <si>
+    <t>Trent Boult</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nTrent Alexander Boult', 'BORN\n\nJuly 22, 1989, Rotorua', 'AGE\n\n35y 351d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nLeft arm Fast medium', 'PLAYING ROLE\n\nBowler', 'RELATIONS\n\nJJ Boult\n\n(brother)']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/trent-boult-277912</t>
+  </si>
+  <si>
+    <t>Jasprit Bumrah</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nJasprit Jasbirsingh Bumrah', 'BORN\n\nDecember 06, 1993, Ahmedabad', 'AGE\n\n31y 214d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nRight arm Fast', 'PLAYING ROLE\n\nBowler']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/jasprit-bumrah-625383</t>
+  </si>
+  <si>
+    <t>Deepak Chahar</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nDeepak Lokandersingh Chahar', 'BORN\n\nAugust 07, 1992, Agra, Uttar Pradesh', 'AGE\n\n32y 335d', 'ALSO KNOWN AS\n\nDeepak Chahar', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nRight arm Medium', 'PLAYING ROLE\n\nBowler', 'RELATIONS\n\nRD Chahar\n\n(cousin)']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/deepak-chahar-447261</t>
+  </si>
+  <si>
+    <t>Richard Gleeson</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nRichard James Gleeson', 'BORN\n\nDecember 02, 1987, Blackpool, Lancashire', 'AGE\n\n37y 218d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nRight arm Fast medium', 'PLAYING ROLE\n\nBowler']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/richard-gleeson-473191</t>
+  </si>
+  <si>
+    <t>Mujeeb Ur Rahman</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nMujeeb Ur Rahman', 'BORN\n\nMarch 28, 2001, Khost', 'AGE\n\n24y 102d', 'ALSO KNOWN AS\n\nMujeeb Zadran', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nRight arm Offbreak', 'PLAYING ROLE\n\nBowler', 'RELATIONS\n\nNoor Ali Zadran\n\n(uncle),\n\nJamshid Zadran\n\n(cousin)']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/mujeeb-ur-rahman-974109</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nPenumatsa Venkata Satyanarayana Raju', 'BORN\n\nJuly 10, 1999', 'AGE\n\n25y 363d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nRight arm Medium fast', 'PLAYING ROLE\n\nBowler', 'RELATIONS\n\nPP Raju\n\n(brother)']</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nKarn Vinod Sharma', 'BORN\n\nOctober 23, 1987, Meerut, Uttar Pradesh', 'AGE\n\n37y 258d', 'BATTING STYLE\n\nLeft hand Bat', 'BOWLING STYLE\n\nLegbreak Googly', 'PLAYING ROLE\n\nBowler']</t>
+  </si>
+  <si>
+    <t>Raghu Sharma</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nRaghu Shivam Sharma', 'BORN\n\nMarch 11, 1993, Jalandhar, Punjab', 'AGE\n\n32y 119d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nLegbreak', 'PLAYING ROLE\n\nBowler']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/raghu-sharma-1122621</t>
+  </si>
+  <si>
+    <t>Arjun Tendulkar</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nArjun Sachin Tendulkar', 'BORN\n\nSeptember 24, 1999, Mumbai', 'AGE\n\n25y 287d', 'BATTING STYLE\n\nLeft hand Bat', 'BOWLING STYLE\n\nLeft arm Medium fast', 'PLAYING ROLE\n\nBowler', 'RELATIONS\n\nSR Tendulkar\n\n(father)']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/arjun-tendulkar-1148776</t>
+  </si>
+  <si>
+    <t>Reece Topley</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nReece James William Topley', 'BORN\n\nFebruary 21, 1994, Ipswich, Suffolk', 'AGE\n\n31y 137d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nLeft arm Fast medium', 'PLAYING ROLE\n\nBowler', 'HEIGHT\n\n6ft 7in', 'RELATIONS\n\nPA Topley\n\n(uncle),\n\nTD Topley\n\n(father)']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/reece-topley-461632</t>
+  </si>
+  <si>
+    <t>AM Ghazanfar</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nAM Ghazanfar', 'BORN\n\nMarch 20, 2006, Paktia', 'AGE\n\n19y 110d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nRight arm Offbreak', 'PLAYING ROLE\n\nBowler']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/am-ghazanfar-1326798</t>
+  </si>
+  <si>
+    <t>Vignesh Puthur</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nVignesh Puthur', 'BORN\n\nMarch 02, 2001', 'AGE\n\n24y 128d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nLeft arm Wrist spin', 'PLAYING ROLE\n\nBowler']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/vignesh-puthur-1460388</t>
+  </si>
+  <si>
+    <t>Lizaad Williams</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nLizaad Buyron Williams', 'BORN\n\nOctober 01, 1993, Vredenburg', 'AGE\n\n31y 280d', 'BATTING STYLE\n\nLeft hand Bat', 'BOWLING STYLE\n\nRight arm Medium fast', 'PLAYING ROLE\n\nBowler']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/lizaad-williams-379887</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nRajat Manohar Patidar', 'BORN\n\nJune 01, 1993, Indore, Madhya Pradesh', 'AGE\n\n32y 37d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nRight arm Offbreak', 'PLAYING ROLE\n\nTop order Batter']</t>
+  </si>
+  <si>
+    <t>Mayank Agarwal</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nMayank Anurag Agarwal', 'BORN\n\nFebruary 16, 1991, Bangalore, Karnataka', 'AGE\n\n34y 142d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nRight arm Offbreak', 'PLAYING ROLE\n\nBatter']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/mayank-agarwal-398438</t>
+  </si>
+  <si>
+    <t>Swastik Chikara</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nSwastik Surender Chikara', 'BORN\n\nApril 03, 2005, Ghaziabad, Uttar Pradesh', 'AGE\n\n20y 96d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nRight arm Offbreak', 'PLAYING ROLE\n\nBatter']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/swastik-chikara-1403198</t>
+  </si>
+  <si>
+    <t>Tim David</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nTimothy Hays David', 'BORN\n\nMarch 16, 1996, Singapore', 'AGE\n\n29y 114d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nRight arm Offbreak', 'PLAYING ROLE\n\nMiddle order Batter', 'HEIGHT\n\n6ft 5in', 'RELATIONS\n\nR David\n\n(father)']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/tim-david-892749</t>
+  </si>
+  <si>
+    <t>Virat Kohli</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nVirat Kohli', 'BORN\n\nNovember 05, 1988, Delhi', 'AGE\n\n36y 245d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nRight arm Medium', 'PLAYING ROLE\n\nTop order Batter']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/virat-kohli-253802</t>
+  </si>
+  <si>
+    <t>Phil Salt</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nPhilip Dean Salt', 'BORN\n\nAugust 28, 1996, Bodelwyddan, North Wales', 'AGE\n\n28y 314d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nRight arm Offbreak', 'FIELDING POSITION\n\nWicketkeeper', 'PLAYING ROLE\n\nWicketkeeper Batter', 'EDUCATION\n\nReeds School, Surrey']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/phil-salt-669365</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nTim Louis Seifert', 'BORN\n\nDecember 14, 1994, Wanganui', 'AGE\n\n30y 206d', 'BATTING STYLE\n\nRight hand Bat', 'FIELDING POSITION\n\nWicketkeeper', 'PLAYING ROLE\n\nWicketkeeper Batter']</t>
+  </si>
+  <si>
+    <t>Jitesh Sharma</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nJitesh Mohan Sharma', 'BORN\n\nOctober 22, 1993, Amrawati, Maharashtra', 'AGE\n\n31y 259d', 'BATTING STYLE\n\nRight hand Bat', 'FIELDING POSITION\n\nWicketkeeper', 'PLAYING ROLE\n\nWicketkeeper Batter']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/jitesh-sharma-721867</t>
+  </si>
+  <si>
+    <t>Devdutt Padikkal</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nDevdutt Padikkal', 'BORN\n\nJuly 07, 2000, Edapal, Kerala', 'AGE\n\n25y 1d', 'BATTING STYLE\n\nLeft hand Bat', 'BOWLING STYLE\n\nRight arm Offbreak', 'PLAYING ROLE\n\nTop order Batter']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/devdutt-padikkal-1119026</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nManoj Shivaramsa Bhandage', 'BORN\n\nOctober 05, 1998, Raichur, Karnataka', 'AGE\n\n26y 276d', 'BATTING STYLE\n\nLeft hand Bat', 'BOWLING STYLE\n\nRight arm Medium fast', 'PLAYING ROLE\n\nAllrounder']</t>
+  </si>
+  <si>
+    <t>Liam Livingstone</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nLiam Stephen Livingstone', 'BORN\n\nAugust 04, 1993, Barrow-in-Furness, Cumberland', 'AGE\n\n31y 338d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nRight arm Offbreak, Legbreak', 'PLAYING ROLE\n\nBatting Allrounder']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/liam-livingstone-403902</t>
+  </si>
+  <si>
+    <t>Mohit Rathee</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nMohit Rathee', 'BORN\n\nJanuary 13, 1999, Rohak, Haryana', 'AGE\n\n26y 176d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nLegbreak', 'PLAYING ROLE\n\nAllrounder']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/mohit-rathee-1349361</t>
+  </si>
+  <si>
+    <t>Krunal Pandya</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nKrunal Himanshu Pandya', 'BORN\n\nMarch 24, 1991, Ahmedabad, Gujarat', 'AGE\n\n34y 106d', 'BATTING STYLE\n\nLeft hand Bat', 'BOWLING STYLE\n\nSlow Left arm Orthodox', 'PLAYING ROLE\n\nAllrounder', 'RELATIONS\n\nHH Pandya\n\n(brother)']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/krunal-pandya-471342</t>
+  </si>
+  <si>
+    <t>Romario Shepherd</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nRomario Shepherd', 'BORN\n\nNovember 26, 1994, Guyana', 'AGE\n\n30y 224d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nRight arm Fast medium', 'PLAYING ROLE\n\nBowling Allrounder']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/romario-shepherd-677077</t>
+  </si>
+  <si>
+    <t>Jacob Bethell</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nJacob Graham Bethell', 'BORN\n\nOctober 23, 2003, Barbados', 'AGE\n\n21y 258d', 'BATTING STYLE\n\nLeft hand Bat', 'BOWLING STYLE\n\nSlow Left arm Orthodox', 'PLAYING ROLE\n\nBatting Allrounder', 'EDUCATION\n\nHarrison College, Barbados; Rugby School']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/jacob-bethell-1194959</t>
+  </si>
+  <si>
+    <t>Abhinandan Singh</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nAbhinandan Singh', 'BORN\n\nMarch 30, 1997', 'AGE\n\n28y 100d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nRight arm Medium fast', 'PLAYING ROLE\n\nBowler']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/abhinandan-singh-1449085</t>
+  </si>
+  <si>
+    <t>Josh Hazlewood</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nJosh Reginald Hazlewood', 'BORN\n\nJanuary 08, 1991, Tamworth, New South Wales', 'AGE\n\n34y 181d', 'BATTING STYLE\n\nLeft hand Bat', 'BOWLING STYLE\n\nRight arm Fast medium', 'PLAYING ROLE\n\nBowler', 'HEIGHT\n\n1.96 m']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/josh-hazlewood-288284</t>
+  </si>
+  <si>
+    <t>Bhuvneshwar Kumar</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nBhuvneshwar Kumar Singh', 'BORN\n\nFebruary 05, 1990, Meerut, Uttar Pradesh', 'AGE\n\n35y 153d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nRight arm Medium', 'PLAYING ROLE\n\nBowler']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/bhuvneshwar-kumar-326016</t>
+  </si>
+  <si>
+    <t>Blessing Muzarabani</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nBlessing Muzarabani', 'BORN\n\nOctober 02, 1996, Harare', 'AGE\n\n28y 279d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nRight arm Fast medium', 'PLAYING ROLE\n\nBowler']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/blessing-muzarabani-827051</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nRasikh Salam Dar', 'BORN\n\nApril 05, 2000', 'AGE\n\n25y 94d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nRight arm Medium', 'PLAYING ROLE\n\nBowler']</t>
+  </si>
+  <si>
+    <t>Suyash Sharma</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nSuyash Sharma', 'BORN\n\nMay 15, 2003', 'AGE\n\n22y 54d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nLegbreak Googly', 'PLAYING ROLE\n\nBowler']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/suyash-sharma-1350792</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nSwapnil Singh', 'BORN\n\nJanuary 22, 1991, Rae Bareilly, Uttar Pradesh', 'AGE\n\n34y 167d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nSlow Left arm Orthodox', 'PLAYING ROLE\n\nBowler']</t>
+  </si>
+  <si>
+    <t>Nuwan Thushara</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nIlandari Dewage Nuwan Thushara', 'BORN\n\nAugust 06, 1994, Thalawa', 'AGE\n\n30y 336d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nRight arm Medium fast', 'PLAYING ROLE\n\nBowler', 'EDUCATION\n\nThalawa Kanitu Vidyalaya, Alpitiya']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/nuwan-thushara-955235</t>
+  </si>
+  <si>
+    <t>Yash Dayal</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nYash Dayal', 'BORN\n\nDecember 13, 1997, Allahabad, Uttar Pradesh', 'AGE\n\n27y 207d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nLeft arm Medium fast', 'PLAYING ROLE\n\nBowler']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/yash-dayal-1159720</t>
+  </si>
+  <si>
+    <t>Lungi Ngidi</t>
+  </si>
+  <si>
+    <t>['FULL NAME\n\nLungisani True-man Ngidi', 'BORN\n\nMarch 29, 1996, Durban, Natal', 'AGE\n\n29y 101d', 'BATTING STYLE\n\nRight hand Bat', 'BOWLING STYLE\n\nRight arm Fast medium', 'PLAYING ROLE\n\nBowler']</t>
+  </si>
+  <si>
+    <t>https://www.espncricinfo.com/cricketers/lungi-ngidi-542023</t>
   </si>
 </sst>
 </file>
@@ -1612,15 +2557,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D133"/>
+  <dimension ref="A1:D238"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="C245" sqref="C245"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
     <col min="2" max="2" width="20.5546875" customWidth="1"/>
-    <col min="3" max="3" width="206.6640625" customWidth="1"/>
+    <col min="3" max="3" width="100.77734375" customWidth="1"/>
     <col min="4" max="4" width="59.5546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2382,1108 +3329,2578 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>165</v>
+        <v>214</v>
       </c>
       <c r="B55" t="s">
-        <v>166</v>
+        <v>215</v>
       </c>
       <c r="C55" t="s">
-        <v>167</v>
+        <v>216</v>
       </c>
       <c r="D55" t="s">
-        <v>168</v>
+        <v>217</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>165</v>
+        <v>214</v>
       </c>
       <c r="B56" t="s">
-        <v>169</v>
+        <v>218</v>
       </c>
       <c r="C56" t="s">
-        <v>170</v>
+        <v>219</v>
       </c>
       <c r="D56" t="s">
-        <v>171</v>
+        <v>220</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>165</v>
+        <v>214</v>
       </c>
       <c r="B57" t="s">
-        <v>172</v>
+        <v>221</v>
       </c>
       <c r="C57" t="s">
-        <v>173</v>
+        <v>222</v>
       </c>
       <c r="D57" t="s">
-        <v>174</v>
+        <v>223</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>165</v>
+        <v>214</v>
       </c>
       <c r="B58" t="s">
-        <v>175</v>
+        <v>224</v>
       </c>
       <c r="C58" t="s">
-        <v>176</v>
+        <v>225</v>
       </c>
       <c r="D58" t="s">
-        <v>177</v>
+        <v>226</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>165</v>
+        <v>214</v>
       </c>
       <c r="B59" t="s">
-        <v>178</v>
+        <v>227</v>
       </c>
       <c r="C59" t="s">
-        <v>179</v>
+        <v>228</v>
       </c>
       <c r="D59" t="s">
-        <v>180</v>
+        <v>229</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>181</v>
+        <v>214</v>
       </c>
       <c r="B60" t="s">
-        <v>182</v>
+        <v>230</v>
       </c>
       <c r="C60" t="s">
-        <v>183</v>
+        <v>231</v>
       </c>
       <c r="D60" t="s">
-        <v>184</v>
+        <v>232</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>181</v>
+        <v>214</v>
       </c>
       <c r="B61" t="s">
-        <v>185</v>
+        <v>233</v>
       </c>
       <c r="C61" t="s">
-        <v>186</v>
+        <v>234</v>
       </c>
       <c r="D61" t="s">
-        <v>187</v>
+        <v>235</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>181</v>
+        <v>214</v>
       </c>
       <c r="B62" t="s">
-        <v>188</v>
+        <v>236</v>
       </c>
       <c r="C62" t="s">
-        <v>189</v>
+        <v>237</v>
       </c>
       <c r="D62" t="s">
-        <v>190</v>
+        <v>238</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>181</v>
+        <v>214</v>
       </c>
       <c r="B63" t="s">
-        <v>191</v>
+        <v>239</v>
       </c>
       <c r="C63" t="s">
-        <v>192</v>
+        <v>240</v>
       </c>
       <c r="D63" t="s">
-        <v>193</v>
+        <v>241</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>181</v>
+        <v>214</v>
       </c>
       <c r="B64" t="s">
-        <v>194</v>
+        <v>242</v>
       </c>
       <c r="C64" t="s">
-        <v>195</v>
+        <v>243</v>
       </c>
       <c r="D64" t="s">
-        <v>196</v>
+        <v>244</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>197</v>
+        <v>214</v>
       </c>
       <c r="B65" t="s">
-        <v>198</v>
+        <v>245</v>
       </c>
       <c r="C65" t="s">
-        <v>199</v>
+        <v>246</v>
       </c>
       <c r="D65" t="s">
-        <v>200</v>
+        <v>247</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>197</v>
+        <v>214</v>
       </c>
       <c r="B66" t="s">
-        <v>201</v>
+        <v>248</v>
       </c>
       <c r="C66" t="s">
-        <v>202</v>
+        <v>249</v>
       </c>
       <c r="D66" t="s">
-        <v>203</v>
+        <v>250</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>197</v>
+        <v>214</v>
       </c>
       <c r="B67" t="s">
-        <v>204</v>
+        <v>251</v>
       </c>
       <c r="C67" t="s">
-        <v>205</v>
+        <v>252</v>
       </c>
       <c r="D67" t="s">
-        <v>206</v>
+        <v>253</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>197</v>
+        <v>214</v>
       </c>
       <c r="B68" t="s">
-        <v>207</v>
+        <v>254</v>
       </c>
       <c r="C68" t="s">
-        <v>208</v>
+        <v>255</v>
       </c>
       <c r="D68" t="s">
-        <v>209</v>
+        <v>256</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>197</v>
+        <v>214</v>
       </c>
       <c r="B69" t="s">
-        <v>210</v>
+        <v>257</v>
       </c>
       <c r="C69" t="s">
-        <v>211</v>
+        <v>258</v>
       </c>
       <c r="D69" t="s">
-        <v>212</v>
+        <v>259</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B70" t="s">
-        <v>214</v>
+        <v>260</v>
       </c>
       <c r="C70" t="s">
-        <v>215</v>
+        <v>261</v>
       </c>
       <c r="D70" t="s">
-        <v>216</v>
+        <v>262</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B71" t="s">
-        <v>217</v>
+        <v>263</v>
       </c>
       <c r="C71" t="s">
-        <v>218</v>
+        <v>264</v>
       </c>
       <c r="D71" t="s">
-        <v>219</v>
+        <v>265</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B72" t="s">
-        <v>220</v>
+        <v>266</v>
       </c>
       <c r="C72" t="s">
-        <v>221</v>
+        <v>267</v>
       </c>
       <c r="D72" t="s">
-        <v>222</v>
+        <v>268</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B73" t="s">
-        <v>223</v>
+        <v>269</v>
       </c>
       <c r="C73" t="s">
-        <v>224</v>
+        <v>270</v>
       </c>
       <c r="D73" t="s">
-        <v>225</v>
+        <v>271</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B74" t="s">
-        <v>226</v>
+        <v>272</v>
       </c>
       <c r="C74" t="s">
-        <v>227</v>
+        <v>273</v>
       </c>
       <c r="D74" t="s">
-        <v>228</v>
+        <v>274</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>229</v>
+        <v>214</v>
       </c>
       <c r="B75" t="s">
-        <v>230</v>
+        <v>275</v>
       </c>
       <c r="C75" t="s">
-        <v>231</v>
+        <v>276</v>
       </c>
       <c r="D75" t="s">
-        <v>232</v>
+        <v>277</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>229</v>
+        <v>214</v>
       </c>
       <c r="B76" t="s">
-        <v>233</v>
+        <v>278</v>
       </c>
       <c r="C76" t="s">
-        <v>234</v>
+        <v>279</v>
       </c>
       <c r="D76" t="s">
-        <v>235</v>
+        <v>280</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>229</v>
+        <v>214</v>
       </c>
       <c r="B77" t="s">
-        <v>236</v>
+        <v>281</v>
       </c>
       <c r="C77" t="s">
-        <v>237</v>
+        <v>282</v>
       </c>
       <c r="D77" t="s">
-        <v>238</v>
+        <v>283</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>229</v>
+        <v>214</v>
       </c>
       <c r="B78" t="s">
-        <v>239</v>
+        <v>284</v>
       </c>
       <c r="C78" t="s">
-        <v>240</v>
+        <v>285</v>
       </c>
       <c r="D78" t="s">
-        <v>241</v>
+        <v>286</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>229</v>
+        <v>214</v>
       </c>
       <c r="B79" t="s">
-        <v>242</v>
+        <v>287</v>
       </c>
       <c r="C79" t="s">
-        <v>243</v>
+        <v>288</v>
       </c>
       <c r="D79" t="s">
-        <v>244</v>
+        <v>289</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>229</v>
+        <v>214</v>
       </c>
       <c r="B80" t="s">
-        <v>245</v>
+        <v>290</v>
       </c>
       <c r="C80" t="s">
-        <v>246</v>
+        <v>291</v>
       </c>
       <c r="D80" t="s">
-        <v>247</v>
+        <v>292</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>229</v>
+        <v>214</v>
       </c>
       <c r="B81" t="s">
-        <v>248</v>
+        <v>293</v>
       </c>
       <c r="C81" t="s">
-        <v>249</v>
+        <v>294</v>
       </c>
       <c r="D81" t="s">
-        <v>250</v>
+        <v>295</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>229</v>
+        <v>296</v>
       </c>
       <c r="B82" t="s">
-        <v>251</v>
+        <v>297</v>
       </c>
       <c r="C82" t="s">
-        <v>252</v>
+        <v>298</v>
       </c>
       <c r="D82" t="s">
-        <v>253</v>
+        <v>299</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>229</v>
+        <v>296</v>
       </c>
       <c r="B83" t="s">
-        <v>254</v>
+        <v>300</v>
       </c>
       <c r="C83" t="s">
-        <v>255</v>
+        <v>301</v>
       </c>
       <c r="D83" t="s">
-        <v>256</v>
+        <v>302</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>229</v>
+        <v>296</v>
       </c>
       <c r="B84" t="s">
-        <v>257</v>
+        <v>303</v>
       </c>
       <c r="C84" t="s">
-        <v>258</v>
+        <v>304</v>
       </c>
       <c r="D84" t="s">
-        <v>259</v>
+        <v>305</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>229</v>
+        <v>296</v>
       </c>
       <c r="B85" t="s">
-        <v>260</v>
+        <v>306</v>
       </c>
       <c r="C85" t="s">
-        <v>261</v>
+        <v>307</v>
       </c>
       <c r="D85" t="s">
-        <v>262</v>
+        <v>308</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>229</v>
+        <v>296</v>
       </c>
       <c r="B86" t="s">
-        <v>263</v>
+        <v>309</v>
       </c>
       <c r="C86" t="s">
-        <v>264</v>
+        <v>310</v>
       </c>
       <c r="D86" t="s">
-        <v>265</v>
+        <v>311</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>229</v>
+        <v>296</v>
       </c>
       <c r="B87" t="s">
-        <v>266</v>
+        <v>312</v>
       </c>
       <c r="C87" t="s">
-        <v>267</v>
+        <v>313</v>
       </c>
       <c r="D87" t="s">
-        <v>268</v>
+        <v>314</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>229</v>
+        <v>296</v>
       </c>
       <c r="B88" t="s">
-        <v>269</v>
+        <v>315</v>
       </c>
       <c r="C88" t="s">
-        <v>270</v>
+        <v>316</v>
       </c>
       <c r="D88" t="s">
-        <v>271</v>
+        <v>317</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>229</v>
+        <v>296</v>
       </c>
       <c r="B89" t="s">
-        <v>272</v>
+        <v>318</v>
       </c>
       <c r="C89" t="s">
-        <v>273</v>
+        <v>319</v>
       </c>
       <c r="D89" t="s">
-        <v>274</v>
+        <v>320</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>229</v>
+        <v>296</v>
       </c>
       <c r="B90" t="s">
-        <v>275</v>
+        <v>321</v>
       </c>
       <c r="C90" t="s">
-        <v>276</v>
+        <v>322</v>
       </c>
       <c r="D90" t="s">
-        <v>277</v>
+        <v>323</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>229</v>
+        <v>296</v>
       </c>
       <c r="B91" t="s">
-        <v>278</v>
+        <v>324</v>
       </c>
       <c r="C91" t="s">
-        <v>279</v>
+        <v>325</v>
       </c>
       <c r="D91" t="s">
-        <v>280</v>
+        <v>326</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>229</v>
+        <v>296</v>
       </c>
       <c r="B92" t="s">
-        <v>281</v>
+        <v>327</v>
       </c>
       <c r="C92" t="s">
-        <v>282</v>
+        <v>328</v>
       </c>
       <c r="D92" t="s">
-        <v>283</v>
+        <v>329</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>229</v>
+        <v>296</v>
       </c>
       <c r="B93" t="s">
-        <v>284</v>
+        <v>330</v>
       </c>
       <c r="C93" t="s">
-        <v>285</v>
+        <v>331</v>
       </c>
       <c r="D93" t="s">
-        <v>286</v>
+        <v>332</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>229</v>
+        <v>296</v>
       </c>
       <c r="B94" t="s">
-        <v>287</v>
+        <v>333</v>
       </c>
       <c r="C94" t="s">
-        <v>288</v>
+        <v>334</v>
       </c>
       <c r="D94" t="s">
-        <v>289</v>
+        <v>335</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>229</v>
+        <v>296</v>
       </c>
       <c r="B95" t="s">
-        <v>290</v>
+        <v>336</v>
       </c>
       <c r="C95" t="s">
-        <v>291</v>
+        <v>337</v>
       </c>
       <c r="D95" t="s">
-        <v>292</v>
+        <v>338</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>229</v>
+        <v>296</v>
       </c>
       <c r="B96" t="s">
-        <v>293</v>
+        <v>339</v>
       </c>
       <c r="C96" t="s">
-        <v>294</v>
+        <v>340</v>
       </c>
       <c r="D96" t="s">
-        <v>295</v>
+        <v>341</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>229</v>
+        <v>296</v>
       </c>
       <c r="B97" t="s">
-        <v>296</v>
+        <v>342</v>
       </c>
       <c r="C97" t="s">
-        <v>297</v>
+        <v>343</v>
       </c>
       <c r="D97" t="s">
-        <v>298</v>
+        <v>344</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>229</v>
+        <v>296</v>
       </c>
       <c r="B98" t="s">
-        <v>299</v>
+        <v>345</v>
       </c>
       <c r="C98" t="s">
-        <v>300</v>
+        <v>346</v>
       </c>
       <c r="D98" t="s">
-        <v>301</v>
+        <v>347</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>229</v>
+        <v>296</v>
       </c>
       <c r="B99" t="s">
-        <v>302</v>
+        <v>348</v>
       </c>
       <c r="C99" t="s">
-        <v>303</v>
+        <v>349</v>
       </c>
       <c r="D99" t="s">
-        <v>304</v>
+        <v>350</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>229</v>
+        <v>296</v>
       </c>
       <c r="B100" t="s">
-        <v>305</v>
+        <v>351</v>
       </c>
       <c r="C100" t="s">
-        <v>306</v>
+        <v>352</v>
       </c>
       <c r="D100" t="s">
-        <v>307</v>
+        <v>353</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>229</v>
+        <v>296</v>
       </c>
       <c r="B101" t="s">
-        <v>308</v>
+        <v>354</v>
       </c>
       <c r="C101" t="s">
-        <v>309</v>
+        <v>355</v>
       </c>
       <c r="D101" t="s">
-        <v>310</v>
+        <v>356</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>311</v>
+        <v>296</v>
       </c>
       <c r="B102" t="s">
-        <v>312</v>
+        <v>357</v>
       </c>
       <c r="C102" t="s">
-        <v>313</v>
+        <v>358</v>
       </c>
       <c r="D102" t="s">
-        <v>314</v>
+        <v>359</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>311</v>
+        <v>296</v>
       </c>
       <c r="B103" t="s">
-        <v>315</v>
+        <v>360</v>
       </c>
       <c r="C103" t="s">
-        <v>316</v>
+        <v>361</v>
       </c>
       <c r="D103" t="s">
-        <v>317</v>
+        <v>362</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>311</v>
+        <v>374</v>
       </c>
       <c r="B104" t="s">
-        <v>318</v>
+        <v>375</v>
       </c>
       <c r="C104" t="s">
-        <v>319</v>
+        <v>376</v>
       </c>
       <c r="D104" t="s">
-        <v>320</v>
+        <v>377</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>311</v>
+        <v>374</v>
       </c>
       <c r="B105" t="s">
-        <v>321</v>
+        <v>378</v>
       </c>
       <c r="C105" t="s">
-        <v>322</v>
+        <v>379</v>
       </c>
       <c r="D105" t="s">
-        <v>323</v>
+        <v>380</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>311</v>
+        <v>374</v>
       </c>
       <c r="B106" t="s">
-        <v>324</v>
+        <v>381</v>
       </c>
       <c r="C106" t="s">
-        <v>325</v>
+        <v>382</v>
       </c>
       <c r="D106" t="s">
-        <v>326</v>
+        <v>383</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>311</v>
+        <v>374</v>
       </c>
       <c r="B107" t="s">
-        <v>327</v>
+        <v>384</v>
       </c>
       <c r="C107" t="s">
-        <v>328</v>
+        <v>385</v>
       </c>
       <c r="D107" t="s">
-        <v>329</v>
+        <v>386</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>311</v>
+        <v>374</v>
       </c>
       <c r="B108" t="s">
-        <v>330</v>
+        <v>387</v>
       </c>
       <c r="C108" t="s">
-        <v>331</v>
+        <v>388</v>
       </c>
       <c r="D108" t="s">
-        <v>332</v>
+        <v>389</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>311</v>
+        <v>176</v>
       </c>
       <c r="B109" t="s">
-        <v>333</v>
+        <v>390</v>
       </c>
       <c r="C109" t="s">
-        <v>334</v>
+        <v>391</v>
       </c>
       <c r="D109" t="s">
-        <v>335</v>
+        <v>392</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>311</v>
+        <v>176</v>
       </c>
       <c r="B110" t="s">
-        <v>336</v>
+        <v>393</v>
       </c>
       <c r="C110" t="s">
-        <v>337</v>
+        <v>394</v>
       </c>
       <c r="D110" t="s">
-        <v>338</v>
+        <v>395</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>311</v>
+        <v>176</v>
       </c>
       <c r="B111" t="s">
-        <v>339</v>
+        <v>396</v>
       </c>
       <c r="C111" t="s">
-        <v>340</v>
+        <v>397</v>
       </c>
       <c r="D111" t="s">
-        <v>341</v>
+        <v>398</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>311</v>
+        <v>176</v>
       </c>
       <c r="B112" t="s">
-        <v>342</v>
+        <v>183</v>
       </c>
       <c r="C112" t="s">
-        <v>343</v>
+        <v>184</v>
       </c>
       <c r="D112" t="s">
-        <v>344</v>
+        <v>185</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>311</v>
+        <v>176</v>
       </c>
       <c r="B113" t="s">
-        <v>345</v>
+        <v>399</v>
       </c>
       <c r="C113" t="s">
-        <v>346</v>
+        <v>400</v>
       </c>
       <c r="D113" t="s">
-        <v>347</v>
+        <v>401</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>311</v>
+        <v>176</v>
       </c>
       <c r="B114" t="s">
-        <v>348</v>
+        <v>402</v>
       </c>
       <c r="C114" t="s">
-        <v>349</v>
+        <v>403</v>
       </c>
       <c r="D114" t="s">
-        <v>350</v>
+        <v>404</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>311</v>
+        <v>176</v>
       </c>
       <c r="B115" t="s">
-        <v>351</v>
+        <v>405</v>
       </c>
       <c r="C115" t="s">
-        <v>352</v>
+        <v>406</v>
       </c>
       <c r="D115" t="s">
-        <v>353</v>
+        <v>407</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>311</v>
+        <v>176</v>
       </c>
       <c r="B116" t="s">
-        <v>354</v>
+        <v>189</v>
       </c>
       <c r="C116" t="s">
-        <v>355</v>
+        <v>190</v>
       </c>
       <c r="D116" t="s">
-        <v>356</v>
+        <v>191</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>311</v>
+        <v>176</v>
       </c>
       <c r="B117" t="s">
-        <v>357</v>
+        <v>408</v>
       </c>
       <c r="C117" t="s">
-        <v>358</v>
+        <v>409</v>
       </c>
       <c r="D117" t="s">
-        <v>359</v>
+        <v>410</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>311</v>
+        <v>176</v>
       </c>
       <c r="B118" t="s">
-        <v>360</v>
+        <v>177</v>
       </c>
       <c r="C118" t="s">
-        <v>361</v>
+        <v>178</v>
       </c>
       <c r="D118" t="s">
-        <v>362</v>
+        <v>179</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>311</v>
+        <v>176</v>
       </c>
       <c r="B119" t="s">
-        <v>363</v>
+        <v>411</v>
       </c>
       <c r="C119" t="s">
-        <v>364</v>
+        <v>412</v>
       </c>
       <c r="D119" t="s">
-        <v>365</v>
+        <v>413</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>311</v>
+        <v>176</v>
       </c>
       <c r="B120" t="s">
-        <v>366</v>
+        <v>186</v>
       </c>
       <c r="C120" t="s">
-        <v>367</v>
+        <v>187</v>
       </c>
       <c r="D120" t="s">
-        <v>368</v>
+        <v>188</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>311</v>
+        <v>176</v>
       </c>
       <c r="B121" t="s">
-        <v>369</v>
+        <v>414</v>
       </c>
       <c r="C121" t="s">
-        <v>370</v>
+        <v>415</v>
       </c>
       <c r="D121" t="s">
-        <v>371</v>
+        <v>416</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>311</v>
+        <v>176</v>
       </c>
       <c r="B122" t="s">
-        <v>372</v>
+        <v>417</v>
       </c>
       <c r="C122" t="s">
-        <v>373</v>
+        <v>418</v>
       </c>
       <c r="D122" t="s">
-        <v>374</v>
+        <v>419</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>311</v>
+        <v>176</v>
       </c>
       <c r="B123" t="s">
-        <v>375</v>
+        <v>420</v>
       </c>
       <c r="C123" t="s">
-        <v>376</v>
+        <v>421</v>
       </c>
       <c r="D123" t="s">
-        <v>377</v>
+        <v>422</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>378</v>
+        <v>176</v>
       </c>
       <c r="B124" t="s">
-        <v>379</v>
+        <v>423</v>
       </c>
       <c r="C124" t="s">
-        <v>380</v>
+        <v>424</v>
       </c>
       <c r="D124" t="s">
-        <v>381</v>
+        <v>425</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>378</v>
+        <v>176</v>
       </c>
       <c r="B125" t="s">
-        <v>382</v>
+        <v>180</v>
       </c>
       <c r="C125" t="s">
-        <v>383</v>
+        <v>181</v>
       </c>
       <c r="D125" t="s">
-        <v>384</v>
+        <v>182</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>378</v>
+        <v>176</v>
       </c>
       <c r="B126" t="s">
-        <v>385</v>
+        <v>426</v>
       </c>
       <c r="C126" t="s">
-        <v>386</v>
+        <v>427</v>
       </c>
       <c r="D126" t="s">
-        <v>387</v>
+        <v>428</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>378</v>
+        <v>176</v>
       </c>
       <c r="B127" t="s">
-        <v>388</v>
+        <v>429</v>
       </c>
       <c r="C127" t="s">
-        <v>389</v>
+        <v>430</v>
       </c>
       <c r="D127" t="s">
-        <v>390</v>
+        <v>431</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>378</v>
+        <v>176</v>
       </c>
       <c r="B128" t="s">
-        <v>391</v>
+        <v>432</v>
       </c>
       <c r="C128" t="s">
-        <v>392</v>
+        <v>433</v>
       </c>
       <c r="D128" t="s">
-        <v>393</v>
+        <v>434</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>394</v>
+        <v>176</v>
       </c>
       <c r="B129" t="s">
-        <v>395</v>
+        <v>435</v>
       </c>
       <c r="C129" t="s">
-        <v>396</v>
+        <v>436</v>
       </c>
       <c r="D129" t="s">
-        <v>397</v>
+        <v>437</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>394</v>
+        <v>176</v>
       </c>
       <c r="B130" t="s">
-        <v>398</v>
+        <v>438</v>
       </c>
       <c r="C130" t="s">
-        <v>399</v>
+        <v>439</v>
       </c>
       <c r="D130" t="s">
-        <v>400</v>
+        <v>440</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>394</v>
+        <v>176</v>
       </c>
       <c r="B131" t="s">
-        <v>401</v>
+        <v>441</v>
       </c>
       <c r="C131" t="s">
-        <v>402</v>
+        <v>442</v>
       </c>
       <c r="D131" t="s">
-        <v>403</v>
+        <v>443</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>394</v>
+        <v>165</v>
       </c>
       <c r="B132" t="s">
-        <v>404</v>
+        <v>444</v>
       </c>
       <c r="C132" t="s">
-        <v>405</v>
+        <v>445</v>
       </c>
       <c r="D132" t="s">
-        <v>406</v>
+        <v>446</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>394</v>
+        <v>165</v>
       </c>
       <c r="B133" t="s">
-        <v>407</v>
+        <v>166</v>
       </c>
       <c r="C133" t="s">
-        <v>408</v>
+        <v>447</v>
       </c>
       <c r="D133" t="s">
-        <v>409</v>
+        <v>167</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A134" t="s">
+        <v>165</v>
+      </c>
+      <c r="B134" t="s">
+        <v>448</v>
+      </c>
+      <c r="C134" t="s">
+        <v>449</v>
+      </c>
+      <c r="D134" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A135" t="s">
+        <v>165</v>
+      </c>
+      <c r="B135" t="s">
+        <v>451</v>
+      </c>
+      <c r="C135" t="s">
+        <v>452</v>
+      </c>
+      <c r="D135" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A136" t="s">
+        <v>165</v>
+      </c>
+      <c r="B136" t="s">
+        <v>454</v>
+      </c>
+      <c r="C136" t="s">
+        <v>455</v>
+      </c>
+      <c r="D136" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A137" t="s">
+        <v>165</v>
+      </c>
+      <c r="B137" t="s">
+        <v>170</v>
+      </c>
+      <c r="C137" t="s">
+        <v>457</v>
+      </c>
+      <c r="D137" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A138" t="s">
+        <v>165</v>
+      </c>
+      <c r="B138" t="s">
+        <v>458</v>
+      </c>
+      <c r="C138" t="s">
+        <v>459</v>
+      </c>
+      <c r="D138" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A139" t="s">
+        <v>165</v>
+      </c>
+      <c r="B139" t="s">
+        <v>461</v>
+      </c>
+      <c r="C139" t="s">
+        <v>462</v>
+      </c>
+      <c r="D139" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A140" t="s">
+        <v>165</v>
+      </c>
+      <c r="B140" t="s">
+        <v>464</v>
+      </c>
+      <c r="C140" t="s">
+        <v>465</v>
+      </c>
+      <c r="D140" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A141" t="s">
+        <v>165</v>
+      </c>
+      <c r="B141" t="s">
+        <v>467</v>
+      </c>
+      <c r="C141" t="s">
+        <v>468</v>
+      </c>
+      <c r="D141" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A142" t="s">
+        <v>165</v>
+      </c>
+      <c r="B142" t="s">
+        <v>168</v>
+      </c>
+      <c r="C142" t="s">
+        <v>470</v>
+      </c>
+      <c r="D142" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A143" t="s">
+        <v>165</v>
+      </c>
+      <c r="B143" t="s">
+        <v>172</v>
+      </c>
+      <c r="C143" t="s">
+        <v>471</v>
+      </c>
+      <c r="D143" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A144" t="s">
+        <v>165</v>
+      </c>
+      <c r="B144" t="s">
+        <v>472</v>
+      </c>
+      <c r="C144" t="s">
+        <v>473</v>
+      </c>
+      <c r="D144" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A145" t="s">
+        <v>165</v>
+      </c>
+      <c r="B145" t="s">
+        <v>475</v>
+      </c>
+      <c r="C145" t="s">
+        <v>476</v>
+      </c>
+      <c r="D145" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A146" t="s">
+        <v>165</v>
+      </c>
+      <c r="B146" t="s">
+        <v>478</v>
+      </c>
+      <c r="C146" t="s">
+        <v>479</v>
+      </c>
+      <c r="D146" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A147" t="s">
+        <v>165</v>
+      </c>
+      <c r="B147" t="s">
+        <v>174</v>
+      </c>
+      <c r="C147" t="s">
+        <v>481</v>
+      </c>
+      <c r="D147" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A148" t="s">
+        <v>165</v>
+      </c>
+      <c r="B148" t="s">
+        <v>482</v>
+      </c>
+      <c r="C148" t="s">
+        <v>483</v>
+      </c>
+      <c r="D148" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A149" t="s">
+        <v>165</v>
+      </c>
+      <c r="B149" t="s">
+        <v>485</v>
+      </c>
+      <c r="C149" t="s">
+        <v>486</v>
+      </c>
+      <c r="D149" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A150" t="s">
+        <v>165</v>
+      </c>
+      <c r="B150" t="s">
+        <v>488</v>
+      </c>
+      <c r="C150" t="s">
+        <v>489</v>
+      </c>
+      <c r="D150" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A151" t="s">
+        <v>165</v>
+      </c>
+      <c r="B151" t="s">
+        <v>491</v>
+      </c>
+      <c r="C151" t="s">
+        <v>492</v>
+      </c>
+      <c r="D151" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A152" t="s">
+        <v>165</v>
+      </c>
+      <c r="B152" t="s">
+        <v>494</v>
+      </c>
+      <c r="C152" t="s">
+        <v>495</v>
+      </c>
+      <c r="D152" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A153" t="s">
+        <v>165</v>
+      </c>
+      <c r="B153" t="s">
+        <v>497</v>
+      </c>
+      <c r="C153" t="s">
+        <v>498</v>
+      </c>
+      <c r="D153" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A154" t="s">
+        <v>165</v>
+      </c>
+      <c r="B154" t="s">
+        <v>500</v>
+      </c>
+      <c r="C154" t="s">
+        <v>501</v>
+      </c>
+      <c r="D154" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A155" t="s">
+        <v>165</v>
+      </c>
+      <c r="B155" t="s">
+        <v>503</v>
+      </c>
+      <c r="C155" t="s">
+        <v>504</v>
+      </c>
+      <c r="D155" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A156" t="s">
+        <v>165</v>
+      </c>
+      <c r="B156" t="s">
+        <v>506</v>
+      </c>
+      <c r="C156" t="s">
+        <v>507</v>
+      </c>
+      <c r="D156" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A157" t="s">
+        <v>165</v>
+      </c>
+      <c r="B157" t="s">
+        <v>509</v>
+      </c>
+      <c r="C157" t="s">
+        <v>510</v>
+      </c>
+      <c r="D157" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A158" t="s">
+        <v>165</v>
+      </c>
+      <c r="B158" t="s">
+        <v>512</v>
+      </c>
+      <c r="C158" t="s">
+        <v>513</v>
+      </c>
+      <c r="D158" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A159" t="s">
+        <v>192</v>
+      </c>
+      <c r="B159" t="s">
+        <v>515</v>
+      </c>
+      <c r="C159" t="s">
+        <v>516</v>
+      </c>
+      <c r="D159" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A160" t="s">
+        <v>192</v>
+      </c>
+      <c r="B160" t="s">
+        <v>518</v>
+      </c>
+      <c r="C160" t="s">
+        <v>519</v>
+      </c>
+      <c r="D160" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A161" t="s">
+        <v>192</v>
+      </c>
+      <c r="B161" t="s">
+        <v>521</v>
+      </c>
+      <c r="C161" t="s">
+        <v>522</v>
+      </c>
+      <c r="D161" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A162" t="s">
+        <v>192</v>
+      </c>
+      <c r="B162" t="s">
+        <v>524</v>
+      </c>
+      <c r="C162" t="s">
+        <v>525</v>
+      </c>
+      <c r="D162" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A163" t="s">
+        <v>192</v>
+      </c>
+      <c r="B163" t="s">
+        <v>527</v>
+      </c>
+      <c r="C163" t="s">
+        <v>528</v>
+      </c>
+      <c r="D163" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A164" t="s">
+        <v>192</v>
+      </c>
+      <c r="B164" t="s">
+        <v>530</v>
+      </c>
+      <c r="C164" t="s">
+        <v>531</v>
+      </c>
+      <c r="D164" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A165" t="s">
+        <v>192</v>
+      </c>
+      <c r="B165" t="s">
+        <v>533</v>
+      </c>
+      <c r="C165" t="s">
+        <v>534</v>
+      </c>
+      <c r="D165" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A166" t="s">
+        <v>192</v>
+      </c>
+      <c r="B166" t="s">
+        <v>536</v>
+      </c>
+      <c r="C166" t="s">
+        <v>537</v>
+      </c>
+      <c r="D166" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A167" t="s">
+        <v>192</v>
+      </c>
+      <c r="B167" t="s">
+        <v>195</v>
+      </c>
+      <c r="C167" t="s">
+        <v>539</v>
+      </c>
+      <c r="D167" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A168" t="s">
+        <v>192</v>
+      </c>
+      <c r="B168" t="s">
+        <v>540</v>
+      </c>
+      <c r="C168" t="s">
+        <v>541</v>
+      </c>
+      <c r="D168" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A169" t="s">
+        <v>192</v>
+      </c>
+      <c r="B169" t="s">
+        <v>197</v>
+      </c>
+      <c r="C169" t="s">
+        <v>543</v>
+      </c>
+      <c r="D169" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A170" t="s">
+        <v>192</v>
+      </c>
+      <c r="B170" t="s">
+        <v>544</v>
+      </c>
+      <c r="C170" t="s">
+        <v>545</v>
+      </c>
+      <c r="D170" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A171" t="s">
+        <v>192</v>
+      </c>
+      <c r="B171" t="s">
+        <v>547</v>
+      </c>
+      <c r="C171" t="s">
+        <v>548</v>
+      </c>
+      <c r="D171" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A172" t="s">
+        <v>192</v>
+      </c>
+      <c r="B172" t="s">
+        <v>550</v>
+      </c>
+      <c r="C172" t="s">
+        <v>551</v>
+      </c>
+      <c r="D172" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A173" t="s">
+        <v>192</v>
+      </c>
+      <c r="B173" t="s">
+        <v>553</v>
+      </c>
+      <c r="C173" t="s">
+        <v>554</v>
+      </c>
+      <c r="D173" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A174" t="s">
+        <v>192</v>
+      </c>
+      <c r="B174" t="s">
+        <v>193</v>
+      </c>
+      <c r="C174" t="s">
+        <v>556</v>
+      </c>
+      <c r="D174" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A175" t="s">
+        <v>192</v>
+      </c>
+      <c r="B175" t="s">
+        <v>557</v>
+      </c>
+      <c r="C175" t="s">
+        <v>558</v>
+      </c>
+      <c r="D175" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A176" t="s">
+        <v>192</v>
+      </c>
+      <c r="B176" t="s">
+        <v>560</v>
+      </c>
+      <c r="C176" t="s">
+        <v>561</v>
+      </c>
+      <c r="D176" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A177" t="s">
+        <v>192</v>
+      </c>
+      <c r="B177" t="s">
+        <v>199</v>
+      </c>
+      <c r="C177" t="s">
+        <v>563</v>
+      </c>
+      <c r="D177" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A178" t="s">
+        <v>192</v>
+      </c>
+      <c r="B178" t="s">
+        <v>564</v>
+      </c>
+      <c r="C178" t="s">
+        <v>565</v>
+      </c>
+      <c r="D178" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A179" t="s">
+        <v>192</v>
+      </c>
+      <c r="B179" t="s">
+        <v>201</v>
+      </c>
+      <c r="C179" t="s">
+        <v>567</v>
+      </c>
+      <c r="D179" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A180" t="s">
+        <v>192</v>
+      </c>
+      <c r="B180" t="s">
+        <v>568</v>
+      </c>
+      <c r="C180" t="s">
+        <v>569</v>
+      </c>
+      <c r="D180" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A181" t="s">
+        <v>192</v>
+      </c>
+      <c r="B181" t="s">
+        <v>571</v>
+      </c>
+      <c r="C181" t="s">
+        <v>572</v>
+      </c>
+      <c r="D181" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A182" t="s">
+        <v>192</v>
+      </c>
+      <c r="B182" t="s">
+        <v>574</v>
+      </c>
+      <c r="C182" t="s">
+        <v>575</v>
+      </c>
+      <c r="D182" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A183" t="s">
+        <v>192</v>
+      </c>
+      <c r="B183" t="s">
+        <v>577</v>
+      </c>
+      <c r="C183" t="s">
+        <v>578</v>
+      </c>
+      <c r="D183" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A184" t="s">
+        <v>192</v>
+      </c>
+      <c r="B184" t="s">
+        <v>580</v>
+      </c>
+      <c r="C184" t="s">
+        <v>581</v>
+      </c>
+      <c r="D184" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A185" t="s">
+        <v>203</v>
+      </c>
+      <c r="B185" t="s">
+        <v>583</v>
+      </c>
+      <c r="C185" t="s">
+        <v>584</v>
+      </c>
+      <c r="D185" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A186" t="s">
+        <v>203</v>
+      </c>
+      <c r="B186" t="s">
+        <v>586</v>
+      </c>
+      <c r="C186" t="s">
+        <v>587</v>
+      </c>
+      <c r="D186" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A187" t="s">
+        <v>203</v>
+      </c>
+      <c r="B187" t="s">
+        <v>589</v>
+      </c>
+      <c r="C187" t="s">
+        <v>590</v>
+      </c>
+      <c r="D187" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A188" t="s">
+        <v>203</v>
+      </c>
+      <c r="B188" t="s">
+        <v>592</v>
+      </c>
+      <c r="C188" t="s">
+        <v>593</v>
+      </c>
+      <c r="D188" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A189" t="s">
+        <v>203</v>
+      </c>
+      <c r="B189" t="s">
+        <v>595</v>
+      </c>
+      <c r="C189" t="s">
+        <v>596</v>
+      </c>
+      <c r="D189" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A190" t="s">
+        <v>203</v>
+      </c>
+      <c r="B190" t="s">
+        <v>598</v>
+      </c>
+      <c r="C190" t="s">
+        <v>599</v>
+      </c>
+      <c r="D190" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A191" t="s">
+        <v>203</v>
+      </c>
+      <c r="B191" t="s">
+        <v>601</v>
+      </c>
+      <c r="C191" t="s">
+        <v>602</v>
+      </c>
+      <c r="D191" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A192" t="s">
+        <v>203</v>
+      </c>
+      <c r="B192" t="s">
+        <v>604</v>
+      </c>
+      <c r="C192" t="s">
+        <v>605</v>
+      </c>
+      <c r="D192" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A193" t="s">
+        <v>203</v>
+      </c>
+      <c r="B193" t="s">
+        <v>607</v>
+      </c>
+      <c r="C193" t="s">
+        <v>608</v>
+      </c>
+      <c r="D193" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A194" t="s">
+        <v>203</v>
+      </c>
+      <c r="B194" t="s">
+        <v>610</v>
+      </c>
+      <c r="C194" t="s">
+        <v>611</v>
+      </c>
+      <c r="D194" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A195" t="s">
+        <v>203</v>
+      </c>
+      <c r="B195" t="s">
+        <v>206</v>
+      </c>
+      <c r="C195" t="s">
+        <v>613</v>
+      </c>
+      <c r="D195" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A196" t="s">
+        <v>203</v>
+      </c>
+      <c r="B196" t="s">
+        <v>614</v>
+      </c>
+      <c r="C196" t="s">
+        <v>615</v>
+      </c>
+      <c r="D196" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A197" t="s">
+        <v>203</v>
+      </c>
+      <c r="B197" t="s">
+        <v>617</v>
+      </c>
+      <c r="C197" t="s">
+        <v>618</v>
+      </c>
+      <c r="D197" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A198" t="s">
+        <v>203</v>
+      </c>
+      <c r="B198" t="s">
+        <v>208</v>
+      </c>
+      <c r="C198" t="s">
+        <v>620</v>
+      </c>
+      <c r="D198" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A199" t="s">
+        <v>203</v>
+      </c>
+      <c r="B199" t="s">
+        <v>621</v>
+      </c>
+      <c r="C199" t="s">
+        <v>622</v>
+      </c>
+      <c r="D199" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A200" t="s">
+        <v>203</v>
+      </c>
+      <c r="B200" t="s">
+        <v>204</v>
+      </c>
+      <c r="C200" t="s">
+        <v>624</v>
+      </c>
+      <c r="D200" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A201" t="s">
+        <v>203</v>
+      </c>
+      <c r="B201" t="s">
+        <v>625</v>
+      </c>
+      <c r="C201" t="s">
+        <v>626</v>
+      </c>
+      <c r="D201" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A202" t="s">
+        <v>203</v>
+      </c>
+      <c r="B202" t="s">
+        <v>628</v>
+      </c>
+      <c r="C202" t="s">
+        <v>629</v>
+      </c>
+      <c r="D202" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A203" t="s">
+        <v>203</v>
+      </c>
+      <c r="B203" t="s">
+        <v>631</v>
+      </c>
+      <c r="C203" t="s">
+        <v>632</v>
+      </c>
+      <c r="D203" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A204" t="s">
+        <v>203</v>
+      </c>
+      <c r="B204" t="s">
+        <v>634</v>
+      </c>
+      <c r="C204" t="s">
+        <v>635</v>
+      </c>
+      <c r="D204" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A205" t="s">
+        <v>203</v>
+      </c>
+      <c r="B205" t="s">
+        <v>637</v>
+      </c>
+      <c r="C205" t="s">
+        <v>638</v>
+      </c>
+      <c r="D205" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A206" t="s">
+        <v>203</v>
+      </c>
+      <c r="B206" t="s">
+        <v>210</v>
+      </c>
+      <c r="C206" t="s">
+        <v>640</v>
+      </c>
+      <c r="D206" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A207" t="s">
+        <v>203</v>
+      </c>
+      <c r="B207" t="s">
+        <v>212</v>
+      </c>
+      <c r="C207" t="s">
+        <v>641</v>
+      </c>
+      <c r="D207" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A208" t="s">
+        <v>203</v>
+      </c>
+      <c r="B208" t="s">
+        <v>642</v>
+      </c>
+      <c r="C208" t="s">
+        <v>643</v>
+      </c>
+      <c r="D208" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A209" t="s">
+        <v>203</v>
+      </c>
+      <c r="B209" t="s">
+        <v>645</v>
+      </c>
+      <c r="C209" t="s">
+        <v>646</v>
+      </c>
+      <c r="D209" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A210" t="s">
+        <v>203</v>
+      </c>
+      <c r="B210" t="s">
+        <v>648</v>
+      </c>
+      <c r="C210" t="s">
+        <v>649</v>
+      </c>
+      <c r="D210" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A211" t="s">
+        <v>203</v>
+      </c>
+      <c r="B211" t="s">
+        <v>651</v>
+      </c>
+      <c r="C211" t="s">
+        <v>652</v>
+      </c>
+      <c r="D211" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A212" t="s">
+        <v>203</v>
+      </c>
+      <c r="B212" t="s">
+        <v>654</v>
+      </c>
+      <c r="C212" t="s">
+        <v>655</v>
+      </c>
+      <c r="D212" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A213" t="s">
+        <v>203</v>
+      </c>
+      <c r="B213" t="s">
+        <v>657</v>
+      </c>
+      <c r="C213" t="s">
+        <v>658</v>
+      </c>
+      <c r="D213" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A214" t="s">
+        <v>363</v>
+      </c>
+      <c r="B214" t="s">
+        <v>366</v>
+      </c>
+      <c r="C214" t="s">
+        <v>660</v>
+      </c>
+      <c r="D214" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A215" t="s">
+        <v>363</v>
+      </c>
+      <c r="B215" t="s">
+        <v>661</v>
+      </c>
+      <c r="C215" t="s">
+        <v>662</v>
+      </c>
+      <c r="D215" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A216" t="s">
+        <v>363</v>
+      </c>
+      <c r="B216" t="s">
+        <v>664</v>
+      </c>
+      <c r="C216" t="s">
+        <v>665</v>
+      </c>
+      <c r="D216" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A217" t="s">
+        <v>363</v>
+      </c>
+      <c r="B217" t="s">
+        <v>667</v>
+      </c>
+      <c r="C217" t="s">
+        <v>668</v>
+      </c>
+      <c r="D217" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A218" t="s">
+        <v>363</v>
+      </c>
+      <c r="B218" t="s">
+        <v>670</v>
+      </c>
+      <c r="C218" t="s">
+        <v>671</v>
+      </c>
+      <c r="D218" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A219" t="s">
+        <v>363</v>
+      </c>
+      <c r="B219" t="s">
+        <v>673</v>
+      </c>
+      <c r="C219" t="s">
+        <v>674</v>
+      </c>
+      <c r="D219" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A220" t="s">
+        <v>363</v>
+      </c>
+      <c r="B220" t="s">
+        <v>370</v>
+      </c>
+      <c r="C220" t="s">
+        <v>676</v>
+      </c>
+      <c r="D220" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A221" t="s">
+        <v>363</v>
+      </c>
+      <c r="B221" t="s">
+        <v>677</v>
+      </c>
+      <c r="C221" t="s">
+        <v>678</v>
+      </c>
+      <c r="D221" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A222" t="s">
+        <v>363</v>
+      </c>
+      <c r="B222" t="s">
+        <v>680</v>
+      </c>
+      <c r="C222" t="s">
+        <v>681</v>
+      </c>
+      <c r="D222" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A223" t="s">
+        <v>363</v>
+      </c>
+      <c r="B223" t="s">
+        <v>364</v>
+      </c>
+      <c r="C223" t="s">
+        <v>683</v>
+      </c>
+      <c r="D223" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A224" t="s">
+        <v>363</v>
+      </c>
+      <c r="B224" t="s">
+        <v>684</v>
+      </c>
+      <c r="C224" t="s">
+        <v>685</v>
+      </c>
+      <c r="D224" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A225" t="s">
+        <v>363</v>
+      </c>
+      <c r="B225" t="s">
+        <v>687</v>
+      </c>
+      <c r="C225" t="s">
+        <v>688</v>
+      </c>
+      <c r="D225" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A226" t="s">
+        <v>363</v>
+      </c>
+      <c r="B226" t="s">
+        <v>690</v>
+      </c>
+      <c r="C226" t="s">
+        <v>691</v>
+      </c>
+      <c r="D226" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A227" t="s">
+        <v>363</v>
+      </c>
+      <c r="B227" t="s">
+        <v>693</v>
+      </c>
+      <c r="C227" t="s">
+        <v>694</v>
+      </c>
+      <c r="D227" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A228" t="s">
+        <v>363</v>
+      </c>
+      <c r="B228" t="s">
+        <v>696</v>
+      </c>
+      <c r="C228" t="s">
+        <v>697</v>
+      </c>
+      <c r="D228" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A229" t="s">
+        <v>363</v>
+      </c>
+      <c r="B229" t="s">
+        <v>699</v>
+      </c>
+      <c r="C229" t="s">
+        <v>700</v>
+      </c>
+      <c r="D229" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A230" t="s">
+        <v>363</v>
+      </c>
+      <c r="B230" t="s">
+        <v>702</v>
+      </c>
+      <c r="C230" t="s">
+        <v>703</v>
+      </c>
+      <c r="D230" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A231" t="s">
+        <v>363</v>
+      </c>
+      <c r="B231" t="s">
+        <v>705</v>
+      </c>
+      <c r="C231" t="s">
+        <v>706</v>
+      </c>
+      <c r="D231" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A232" t="s">
+        <v>363</v>
+      </c>
+      <c r="B232" t="s">
+        <v>708</v>
+      </c>
+      <c r="C232" t="s">
+        <v>709</v>
+      </c>
+      <c r="D232" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A233" t="s">
+        <v>363</v>
+      </c>
+      <c r="B233" t="s">
+        <v>368</v>
+      </c>
+      <c r="C233" t="s">
+        <v>711</v>
+      </c>
+      <c r="D233" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A234" t="s">
+        <v>363</v>
+      </c>
+      <c r="B234" t="s">
+        <v>712</v>
+      </c>
+      <c r="C234" t="s">
+        <v>713</v>
+      </c>
+      <c r="D234" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A235" t="s">
+        <v>363</v>
+      </c>
+      <c r="B235" t="s">
+        <v>372</v>
+      </c>
+      <c r="C235" t="s">
+        <v>715</v>
+      </c>
+      <c r="D235" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A236" t="s">
+        <v>363</v>
+      </c>
+      <c r="B236" t="s">
+        <v>716</v>
+      </c>
+      <c r="C236" t="s">
+        <v>717</v>
+      </c>
+      <c r="D236" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A237" t="s">
+        <v>363</v>
+      </c>
+      <c r="B237" t="s">
+        <v>719</v>
+      </c>
+      <c r="C237" t="s">
+        <v>720</v>
+      </c>
+      <c r="D237" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="238" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A238" t="s">
+        <v>363</v>
+      </c>
+      <c r="B238" t="s">
+        <v>722</v>
+      </c>
+      <c r="C238" t="s">
+        <v>723</v>
+      </c>
+      <c r="D238" t="s">
+        <v>724</v>
       </c>
     </row>
   </sheetData>

</xml_diff>